<commit_message>
Completed Invoice layout version 1.0
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{55225790-E440-4FF5-A4B0-DE1DBAFF81DC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{41D10F38-AA9E-4E5C-8F25-6BBB17517380}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{AFF0B8A1-9626-46B3-9A62-F42AFA134D79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="114">
   <si>
     <t>Test Case</t>
   </si>
@@ -325,6 +325,48 @@
   </si>
   <si>
     <t>Record should be displayed because the customer list grid will pull customers that do not yet have contacts associated with them.</t>
+  </si>
+  <si>
+    <t>Select an existing customer (Click on their name)</t>
+  </si>
+  <si>
+    <t>The Customer Details window should be displayed</t>
+  </si>
+  <si>
+    <t>Under the Address Section, click on the 'Add' link</t>
+  </si>
+  <si>
+    <t>A new Address entry should be displayed at the top of the section</t>
+  </si>
+  <si>
+    <t>Add a new Address that is different from the existing (Either Billing, Shipping or Other)</t>
+  </si>
+  <si>
+    <t>Screen should allow for entry of values</t>
+  </si>
+  <si>
+    <t>Bring up Customer Details screen again</t>
+  </si>
+  <si>
+    <t>The Customer Details window should display.  The new address should be displayed</t>
+  </si>
+  <si>
+    <t>Under the Contacts Section, click on the 'Add' link</t>
+  </si>
+  <si>
+    <t>A new Contacts entry should be displayed at the top of the section</t>
+  </si>
+  <si>
+    <t>Add a new Contact that is different from the existing (Either Primary, Secondary, or Other))</t>
+  </si>
+  <si>
+    <t>The Customer Details window should display.  The new contact should be displayed</t>
+  </si>
+  <si>
+    <t>Edit customer information (Name, etc.)</t>
+  </si>
+  <si>
+    <t>All fields should be editable except for the Setup Date and Setup By values.</t>
   </si>
 </sst>
 </file>
@@ -1208,10 +1250,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H177"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2350,227 +2392,253 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="13">
         <v>1</v>
       </c>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="E65" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="G65" s="29"/>
       <c r="H65" s="16"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="13">
         <v>2</v>
       </c>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
+      <c r="E66" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="G66" s="29"/>
       <c r="H66" s="16"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
       <c r="D67" s="13">
         <v>3</v>
       </c>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
+      <c r="E67" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>103</v>
+      </c>
       <c r="G67" s="29"/>
       <c r="H67" s="16"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="13">
+        <v>4</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G68" s="29"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="13">
+        <v>5</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="G69" s="29"/>
+      <c r="H69" s="16"/>
+    </row>
+    <row r="70" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="13">
+        <v>6</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F70" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G70" s="29"/>
+      <c r="H70" s="16"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="30" t="s">
+      <c r="B71" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="30"/>
-      <c r="E68" s="31" t="s">
+      <c r="D71" s="30"/>
+      <c r="E71" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A69" s="6">
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
         <v>11</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D69" s="27"/>
-      <c r="E69" s="7" t="s">
+      <c r="D72" s="27"/>
+      <c r="E72" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="16"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F70" s="11" t="s">
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="16"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H70" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="13">
-        <v>1</v>
-      </c>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="16"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="13">
-        <v>2</v>
-      </c>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="16"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="13">
-        <v>3</v>
-      </c>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
-      <c r="G73" s="29"/>
-      <c r="H73" s="16"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" s="30"/>
-      <c r="E74" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="33" t="s">
-        <v>6</v>
-      </c>
+      <c r="H73" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="13">
+        <v>1</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F74" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G74" s="29"/>
+      <c r="H74" s="16"/>
     </row>
     <row r="75" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="6">
-        <v>12</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D75" s="27"/>
-      <c r="E75" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="13">
+        <v>2</v>
+      </c>
+      <c r="E75" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F75" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G75" s="29"/>
       <c r="H75" s="16"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="22"/>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H76" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="13">
+        <v>3</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F76" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="G76" s="29"/>
+      <c r="H76" s="16"/>
+    </row>
+    <row r="77" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
       <c r="D77" s="13">
-        <v>1</v>
-      </c>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
+        <v>4</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F77" s="29" t="s">
+        <v>105</v>
+      </c>
       <c r="G77" s="29"/>
       <c r="H77" s="16"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
       <c r="D78" s="13">
-        <v>2</v>
-      </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
+        <v>5</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F78" s="29" t="s">
+        <v>94</v>
+      </c>
       <c r="G78" s="29"/>
       <c r="H78" s="16"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="D79" s="13">
-        <v>3</v>
-      </c>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
+        <v>6</v>
+      </c>
+      <c r="E79" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F79" s="29" t="s">
+        <v>111</v>
+      </c>
       <c r="G79" s="29"/>
       <c r="H79" s="16"/>
     </row>
@@ -2596,7 +2664,7 @@
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>7</v>
@@ -2606,7 +2674,7 @@
       </c>
       <c r="D81" s="27"/>
       <c r="E81" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F81" s="28"/>
       <c r="G81" s="28"/>
@@ -2632,595 +2700,581 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
       <c r="D83" s="13">
         <v>1</v>
       </c>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
+      <c r="E83" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F83" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="G83" s="29"/>
       <c r="H83" s="16"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
       <c r="D84" s="13">
         <v>2</v>
       </c>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
+      <c r="E84" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F84" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="G84" s="29"/>
       <c r="H84" s="16"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
       <c r="D85" s="13">
         <v>3</v>
       </c>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
+      <c r="E85" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F85" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="G85" s="29"/>
       <c r="H85" s="16"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="30" t="s">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="13">
+        <v>4</v>
+      </c>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="16"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="13">
+        <v>5</v>
+      </c>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="16"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="16"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="30" t="s">
+      <c r="B89" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D86" s="30"/>
-      <c r="E86" s="31" t="s">
+      <c r="D89" s="30"/>
+      <c r="E89" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F86" s="31"/>
-      <c r="G86" s="31"/>
-      <c r="H86" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A87" s="6">
+      <c r="F89" s="31"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>13</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D90" s="27"/>
+      <c r="E90" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="16"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="22"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H91" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="13">
+        <v>1</v>
+      </c>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="16"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="13">
+        <v>2</v>
+      </c>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="16"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="13">
+        <v>3</v>
+      </c>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="16"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" s="30"/>
+      <c r="E95" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F95" s="31"/>
+      <c r="G95" s="31"/>
+      <c r="H95" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
         <v>14</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B96" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C96" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D87" s="27"/>
-      <c r="E87" s="7" t="s">
+      <c r="D96" s="27"/>
+      <c r="E96" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F87" s="28"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="16"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="22"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F88" s="11" t="s">
+      <c r="F96" s="28"/>
+      <c r="G96" s="28"/>
+      <c r="H96" s="16"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="22"/>
+      <c r="B97" s="22"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E97" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F97" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G88" s="11" t="s">
+      <c r="G97" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H88" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="14"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="13">
-        <v>1</v>
-      </c>
-      <c r="E89" s="29"/>
-      <c r="F89" s="29"/>
-      <c r="G89" s="29"/>
-      <c r="H89" s="16"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="14"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="13">
-        <v>2</v>
-      </c>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="16"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="13">
-        <v>3</v>
-      </c>
-      <c r="E91" s="29"/>
-      <c r="F91" s="29"/>
-      <c r="G91" s="29"/>
-      <c r="H91" s="16"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="30" t="s">
+      <c r="H97" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="13">
+        <v>1</v>
+      </c>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
+      <c r="H98" s="16"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="13">
+        <v>2</v>
+      </c>
+      <c r="E99" s="29"/>
+      <c r="F99" s="29"/>
+      <c r="G99" s="29"/>
+      <c r="H99" s="16"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="13">
+        <v>3</v>
+      </c>
+      <c r="E100" s="29"/>
+      <c r="F100" s="29"/>
+      <c r="G100" s="29"/>
+      <c r="H100" s="16"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B92" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="30" t="s">
+      <c r="B101" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D92" s="30"/>
-      <c r="E92" s="31" t="s">
+      <c r="D101" s="30"/>
+      <c r="E101" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F92" s="31"/>
-      <c r="G92" s="31"/>
-      <c r="H92" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="6">
+      <c r="F101" s="31"/>
+      <c r="G101" s="31"/>
+      <c r="H101" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
         <v>15</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B102" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C102" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D93" s="27"/>
-      <c r="E93" s="7" t="s">
+      <c r="D102" s="27"/>
+      <c r="E102" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F93" s="28"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="16"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="22"/>
-      <c r="B94" s="22"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F94" s="11" t="s">
+      <c r="F102" s="28"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="16"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="22"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F103" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G94" s="11" t="s">
+      <c r="G103" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H94" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="13">
-        <v>1</v>
-      </c>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="16"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="13">
-        <v>2</v>
-      </c>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
-      <c r="G96" s="29"/>
-      <c r="H96" s="16"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="14"/>
-      <c r="B97" s="14"/>
-      <c r="C97" s="14"/>
-      <c r="D97" s="13">
-        <v>3</v>
-      </c>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
-      <c r="G97" s="29"/>
-      <c r="H97" s="16"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="30" t="s">
+      <c r="H103" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="13">
+        <v>1</v>
+      </c>
+      <c r="E104" s="29"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="29"/>
+      <c r="H104" s="16"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="13">
+        <v>2</v>
+      </c>
+      <c r="E105" s="29"/>
+      <c r="F105" s="29"/>
+      <c r="G105" s="29"/>
+      <c r="H105" s="16"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="13">
+        <v>3</v>
+      </c>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="29"/>
+      <c r="H106" s="16"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B98" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="30" t="s">
+      <c r="B107" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D98" s="30"/>
-      <c r="E98" s="31" t="s">
+      <c r="D107" s="30"/>
+      <c r="E107" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F98" s="31"/>
-      <c r="G98" s="31"/>
-      <c r="H98" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A99" s="6">
+      <c r="F107" s="31"/>
+      <c r="G107" s="31"/>
+      <c r="H107" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A108" s="6">
         <v>16</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="B108" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="C108" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D99" s="27"/>
-      <c r="E99" s="7" t="s">
+      <c r="D108" s="27"/>
+      <c r="E108" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F99" s="28"/>
-      <c r="G99" s="28"/>
-      <c r="H99" s="16"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="22"/>
-      <c r="B100" s="22"/>
-      <c r="C100" s="22"/>
-      <c r="D100" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F100" s="11" t="s">
+      <c r="F108" s="28"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="16"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="22"/>
+      <c r="B109" s="22"/>
+      <c r="C109" s="22"/>
+      <c r="D109" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E109" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F109" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G100" s="11" t="s">
+      <c r="G109" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H100" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="14"/>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
-      <c r="D101" s="13">
-        <v>1</v>
-      </c>
-      <c r="E101" s="29"/>
-      <c r="F101" s="29"/>
-      <c r="G101" s="29"/>
-      <c r="H101" s="16"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="14"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
-      <c r="D102" s="13">
-        <v>2</v>
-      </c>
-      <c r="E102" s="29"/>
-      <c r="F102" s="29"/>
-      <c r="G102" s="29"/>
-      <c r="H102" s="16"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="14"/>
-      <c r="D103" s="13">
-        <v>3</v>
-      </c>
-      <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
-      <c r="G103" s="29"/>
-      <c r="H103" s="16"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="30" t="s">
+      <c r="H109" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="14"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="13">
+        <v>1</v>
+      </c>
+      <c r="E110" s="29"/>
+      <c r="F110" s="29"/>
+      <c r="G110" s="29"/>
+      <c r="H110" s="16"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="13">
+        <v>2</v>
+      </c>
+      <c r="E111" s="29"/>
+      <c r="F111" s="29"/>
+      <c r="G111" s="29"/>
+      <c r="H111" s="16"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="13">
+        <v>3</v>
+      </c>
+      <c r="E112" s="29"/>
+      <c r="F112" s="29"/>
+      <c r="G112" s="29"/>
+      <c r="H112" s="16"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B104" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="30" t="s">
+      <c r="B113" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D104" s="30"/>
-      <c r="E104" s="31" t="s">
+      <c r="D113" s="30"/>
+      <c r="E113" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F104" s="31"/>
-      <c r="G104" s="31"/>
-      <c r="H104" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A105" s="6">
+      <c r="F113" s="31"/>
+      <c r="G113" s="31"/>
+      <c r="H113" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A114" s="6">
         <v>17</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B114" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C105" s="6" t="s">
+      <c r="C114" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D105" s="27"/>
-      <c r="E105" s="7" t="s">
+      <c r="D114" s="27"/>
+      <c r="E114" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F105" s="28"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="16"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="22"/>
-      <c r="B106" s="22"/>
-      <c r="C106" s="22"/>
-      <c r="D106" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F106" s="11" t="s">
+      <c r="F114" s="28"/>
+      <c r="G114" s="28"/>
+      <c r="H114" s="16"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="22"/>
+      <c r="B115" s="22"/>
+      <c r="C115" s="22"/>
+      <c r="D115" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F115" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G106" s="11" t="s">
+      <c r="G115" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H106" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
-      <c r="D107" s="13">
-        <v>1</v>
-      </c>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="16"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="14"/>
-      <c r="D108" s="13">
-        <v>2</v>
-      </c>
-      <c r="E108" s="29"/>
-      <c r="F108" s="29"/>
-      <c r="G108" s="29"/>
-      <c r="H108" s="16"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="13">
-        <v>3</v>
-      </c>
-      <c r="E109" s="29"/>
-      <c r="F109" s="29"/>
-      <c r="G109" s="29"/>
-      <c r="H109" s="16"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D110" s="25"/>
-      <c r="E110" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F110" s="26"/>
-      <c r="G110" s="26"/>
-      <c r="H110" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A111" s="6">
-        <v>18</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D111" s="27"/>
-      <c r="E111" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F111" s="28"/>
-      <c r="G111" s="28"/>
-      <c r="H111" s="16"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="22"/>
-      <c r="B112" s="22"/>
-      <c r="C112" s="22"/>
-      <c r="D112" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E112" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F112" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G112" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H112" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A113" s="14"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="13">
-        <v>1</v>
-      </c>
-      <c r="E113" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F113" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G113" s="23"/>
-      <c r="H113" s="16"/>
-    </row>
-    <row r="114" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="13">
-        <v>2</v>
-      </c>
-      <c r="E114" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F114" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G114" s="23"/>
-      <c r="H114" s="16"/>
-    </row>
-    <row r="115" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A115" s="14"/>
-      <c r="B115" s="14"/>
-      <c r="C115" s="14"/>
-      <c r="D115" s="13">
-        <v>3</v>
-      </c>
-      <c r="E115" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F115" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G115" s="23"/>
-      <c r="H115" s="16"/>
-    </row>
-    <row r="116" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="H115" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="14"/>
       <c r="B116" s="14"/>
       <c r="C116" s="14"/>
       <c r="D116" s="13">
-        <v>3</v>
-      </c>
-      <c r="E116" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="F116" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="G116" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="29"/>
       <c r="H116" s="16"/>
     </row>
-    <row r="117" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="14"/>
       <c r="B117" s="14"/>
       <c r="C117" s="14"/>
       <c r="D117" s="13">
-        <v>4</v>
-      </c>
-      <c r="E117" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="F117" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="G117" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
       <c r="H117" s="16"/>
     </row>
-    <row r="118" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="14"/>
       <c r="B118" s="14"/>
       <c r="C118" s="14"/>
       <c r="D118" s="13">
-        <v>5</v>
-      </c>
-      <c r="E118" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="F118" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="G118" s="23"/>
+        <v>3</v>
+      </c>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
+      <c r="G118" s="29"/>
       <c r="H118" s="16"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="30" t="s">
+      <c r="A119" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B119" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="30" t="s">
+      <c r="B119" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D119" s="30"/>
-      <c r="E119" s="31" t="s">
+      <c r="D119" s="25"/>
+      <c r="E119" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F119" s="31"/>
-      <c r="G119" s="31"/>
+      <c r="F119" s="26"/>
+      <c r="G119" s="26"/>
       <c r="H119" s="33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>7</v>
@@ -3230,7 +3284,7 @@
       </c>
       <c r="D120" s="27"/>
       <c r="E120" s="7" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F120" s="28"/>
       <c r="G120" s="28"/>
@@ -3304,506 +3358,550 @@
       <c r="G124" s="23"/>
       <c r="H124" s="16"/>
     </row>
-    <row r="125" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A125" s="14"/>
       <c r="B125" s="14"/>
       <c r="C125" s="14"/>
       <c r="D125" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E125" s="29" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="F125" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G125" s="29"/>
+        <v>38</v>
+      </c>
+      <c r="G125" s="23"/>
       <c r="H125" s="16"/>
     </row>
-    <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A126" s="14"/>
       <c r="B126" s="14"/>
       <c r="C126" s="14"/>
       <c r="D126" s="13">
+        <v>4</v>
+      </c>
+      <c r="E126" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F126" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G126" s="23"/>
+      <c r="H126" s="16"/>
+    </row>
+    <row r="127" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A127" s="14"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="13">
         <v>5</v>
       </c>
-      <c r="E126" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F126" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="G126" s="29"/>
-      <c r="H126" s="16"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="30" t="s">
+      <c r="E127" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F127" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G127" s="23"/>
+      <c r="H127" s="16"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B127" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="30" t="s">
+      <c r="B128" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D127" s="30"/>
-      <c r="E127" s="31" t="s">
+      <c r="D128" s="30"/>
+      <c r="E128" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F127" s="31"/>
-      <c r="G127" s="31"/>
-      <c r="H127" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A128" s="6">
-        <v>20</v>
-      </c>
-      <c r="B128" s="6" t="s">
+      <c r="F128" s="31"/>
+      <c r="G128" s="31"/>
+      <c r="H128" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A129" s="6">
+        <v>19</v>
+      </c>
+      <c r="B129" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C128" s="6" t="s">
+      <c r="C129" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D128" s="27"/>
-      <c r="E128" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F128" s="28"/>
-      <c r="G128" s="28"/>
-      <c r="H128" s="16"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="22"/>
-      <c r="B129" s="22"/>
-      <c r="C129" s="22"/>
-      <c r="D129" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E129" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F129" s="11" t="s">
+      <c r="D129" s="27"/>
+      <c r="E129" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F129" s="28"/>
+      <c r="G129" s="28"/>
+      <c r="H129" s="16"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="22"/>
+      <c r="B130" s="22"/>
+      <c r="C130" s="22"/>
+      <c r="D130" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E130" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F130" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G129" s="11" t="s">
+      <c r="G130" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H129" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A130" s="14"/>
-      <c r="B130" s="14"/>
-      <c r="C130" s="14"/>
-      <c r="D130" s="13">
-        <v>1</v>
-      </c>
-      <c r="E130" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F130" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G130" s="23"/>
-      <c r="H130" s="16"/>
-    </row>
-    <row r="131" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="H130" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A131" s="14"/>
       <c r="B131" s="14"/>
       <c r="C131" s="14"/>
       <c r="D131" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E131" s="29" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F131" s="29" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="G131" s="23"/>
       <c r="H131" s="16"/>
     </row>
-    <row r="132" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A132" s="14"/>
       <c r="B132" s="14"/>
       <c r="C132" s="14"/>
       <c r="D132" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E132" s="29" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F132" s="29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G132" s="23"/>
       <c r="H132" s="16"/>
     </row>
-    <row r="133" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A133" s="14"/>
       <c r="B133" s="14"/>
       <c r="C133" s="14"/>
       <c r="D133" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E133" s="29" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="F133" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="G133" s="29"/>
+        <v>85</v>
+      </c>
+      <c r="G133" s="23"/>
       <c r="H133" s="16"/>
     </row>
-    <row r="134" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A134" s="14"/>
       <c r="B134" s="14"/>
       <c r="C134" s="14"/>
       <c r="D134" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="F134" s="29" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G134" s="29"/>
       <c r="H134" s="16"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="30" t="s">
+    <row r="135" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A135" s="14"/>
+      <c r="B135" s="14"/>
+      <c r="C135" s="14"/>
+      <c r="D135" s="13">
+        <v>5</v>
+      </c>
+      <c r="E135" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F135" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G135" s="29"/>
+      <c r="H135" s="16"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B135" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C135" s="30" t="s">
+      <c r="B136" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D135" s="30"/>
-      <c r="E135" s="31" t="s">
+      <c r="D136" s="30"/>
+      <c r="E136" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F135" s="31"/>
-      <c r="G135" s="31"/>
-      <c r="H135" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A136" s="6">
-        <v>21</v>
-      </c>
-      <c r="B136" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136" s="6" t="s">
+      <c r="F136" s="31"/>
+      <c r="G136" s="31"/>
+      <c r="H136" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A137" s="6">
+        <v>20</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D136" s="27"/>
-      <c r="E136" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F136" s="28"/>
-      <c r="G136" s="28"/>
-      <c r="H136" s="16"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="22"/>
-      <c r="B137" s="22"/>
-      <c r="C137" s="22"/>
-      <c r="D137" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E137" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F137" s="11" t="s">
+      <c r="D137" s="27"/>
+      <c r="E137" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F137" s="28"/>
+      <c r="G137" s="28"/>
+      <c r="H137" s="16"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" s="22"/>
+      <c r="B138" s="22"/>
+      <c r="C138" s="22"/>
+      <c r="D138" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E138" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F138" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G137" s="11" t="s">
+      <c r="G138" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H137" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="14"/>
-      <c r="B138" s="14"/>
-      <c r="C138" s="14"/>
-      <c r="D138" s="13">
-        <v>1</v>
-      </c>
-      <c r="E138" s="29"/>
-      <c r="F138" s="29"/>
-      <c r="G138" s="29"/>
-      <c r="H138" s="16"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H138" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A139" s="14"/>
       <c r="B139" s="14"/>
       <c r="C139" s="14"/>
       <c r="D139" s="13">
-        <v>2</v>
-      </c>
-      <c r="E139" s="29"/>
-      <c r="F139" s="29"/>
-      <c r="G139" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="E139" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F139" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G139" s="23"/>
       <c r="H139" s="16"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A140" s="14"/>
       <c r="B140" s="14"/>
       <c r="C140" s="14"/>
       <c r="D140" s="13">
-        <v>3</v>
-      </c>
-      <c r="E140" s="29"/>
-      <c r="F140" s="29"/>
-      <c r="G140" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="E140" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F140" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G140" s="23"/>
       <c r="H140" s="16"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="30" t="s">
+    <row r="141" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A141" s="14"/>
+      <c r="B141" s="14"/>
+      <c r="C141" s="14"/>
+      <c r="D141" s="13">
+        <v>3</v>
+      </c>
+      <c r="E141" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F141" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G141" s="23"/>
+      <c r="H141" s="16"/>
+    </row>
+    <row r="142" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="14"/>
+      <c r="D142" s="13">
+        <v>2</v>
+      </c>
+      <c r="E142" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F142" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G142" s="29"/>
+      <c r="H142" s="16"/>
+    </row>
+    <row r="143" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A143" s="14"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="14"/>
+      <c r="D143" s="13">
+        <v>3</v>
+      </c>
+      <c r="E143" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F143" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G143" s="29"/>
+      <c r="H143" s="16"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B141" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C141" s="30" t="s">
+      <c r="B144" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D141" s="30"/>
-      <c r="E141" s="31" t="s">
+      <c r="D144" s="30"/>
+      <c r="E144" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F141" s="31"/>
-      <c r="G141" s="31"/>
-      <c r="H141" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A142" s="6">
-        <v>22</v>
-      </c>
-      <c r="B142" s="6" t="s">
+      <c r="F144" s="31"/>
+      <c r="G144" s="31"/>
+      <c r="H144" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A145" s="6">
+        <v>21</v>
+      </c>
+      <c r="B145" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C142" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D142" s="27"/>
-      <c r="E142" s="7" t="s">
+      <c r="C145" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D145" s="27"/>
+      <c r="E145" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F142" s="28"/>
-      <c r="G142" s="28"/>
-      <c r="H142" s="16"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A143" s="22"/>
-      <c r="B143" s="22"/>
-      <c r="C143" s="22"/>
-      <c r="D143" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E143" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F143" s="11" t="s">
+      <c r="F145" s="28"/>
+      <c r="G145" s="28"/>
+      <c r="H145" s="16"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="22"/>
+      <c r="B146" s="22"/>
+      <c r="C146" s="22"/>
+      <c r="D146" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E146" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F146" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G143" s="11" t="s">
+      <c r="G146" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H143" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="14"/>
-      <c r="B144" s="14"/>
-      <c r="C144" s="14"/>
-      <c r="D144" s="13">
-        <v>1</v>
-      </c>
-      <c r="E144" s="29"/>
-      <c r="F144" s="29"/>
-      <c r="G144" s="29"/>
-      <c r="H144" s="16"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A145" s="14"/>
-      <c r="B145" s="14"/>
-      <c r="C145" s="14"/>
-      <c r="D145" s="13">
-        <v>2</v>
-      </c>
-      <c r="E145" s="29"/>
-      <c r="F145" s="29"/>
-      <c r="G145" s="29"/>
-      <c r="H145" s="16"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A146" s="14"/>
-      <c r="B146" s="14"/>
-      <c r="C146" s="14"/>
-      <c r="D146" s="13">
-        <v>3</v>
-      </c>
-      <c r="E146" s="29"/>
-      <c r="F146" s="29"/>
-      <c r="G146" s="29"/>
-      <c r="H146" s="16"/>
+      <c r="H146" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="14"/>
       <c r="B147" s="14"/>
       <c r="C147" s="14"/>
-      <c r="D147" s="13"/>
+      <c r="D147" s="13">
+        <v>1</v>
+      </c>
       <c r="E147" s="29"/>
       <c r="F147" s="29"/>
       <c r="G147" s="29"/>
-      <c r="H147" s="13"/>
+      <c r="H147" s="16"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="14"/>
       <c r="B148" s="14"/>
       <c r="C148" s="14"/>
-      <c r="D148" s="13"/>
+      <c r="D148" s="13">
+        <v>2</v>
+      </c>
       <c r="E148" s="29"/>
       <c r="F148" s="29"/>
       <c r="G148" s="29"/>
-      <c r="H148" s="13"/>
+      <c r="H148" s="16"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="14"/>
       <c r="B149" s="14"/>
       <c r="C149" s="14"/>
-      <c r="D149" s="13"/>
+      <c r="D149" s="13">
+        <v>3</v>
+      </c>
       <c r="E149" s="29"/>
       <c r="F149" s="29"/>
       <c r="G149" s="29"/>
-      <c r="H149" s="13"/>
+      <c r="H149" s="16"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A150" s="14"/>
-      <c r="B150" s="14"/>
-      <c r="C150" s="14"/>
-      <c r="D150" s="14"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="15"/>
-      <c r="G150" s="15"/>
-      <c r="H150" s="14"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A151" s="14">
+      <c r="A150" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B150" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D150" s="30"/>
+      <c r="E150" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F150" s="31"/>
+      <c r="G150" s="31"/>
+      <c r="H150" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A151" s="6">
+        <v>22</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D151" s="27"/>
+      <c r="E151" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F151" s="28"/>
+      <c r="G151" s="28"/>
+      <c r="H151" s="16"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="22"/>
+      <c r="B152" s="22"/>
+      <c r="C152" s="22"/>
+      <c r="D152" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E152" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F152" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G152" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B151" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C151" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D151" s="14"/>
-      <c r="E151" s="15"/>
-      <c r="F151" s="15"/>
-      <c r="G151" s="15"/>
-      <c r="H151" s="14"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A152" s="14"/>
-      <c r="B152" s="14"/>
-      <c r="C152" s="14"/>
-      <c r="D152" s="14"/>
-      <c r="E152" s="15"/>
-      <c r="F152" s="15"/>
-      <c r="G152" s="15"/>
-      <c r="H152" s="14"/>
+      <c r="H152" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A153" s="14">
-        <v>7</v>
-      </c>
+      <c r="A153" s="14"/>
       <c r="B153" s="14"/>
       <c r="C153" s="14"/>
-      <c r="D153" s="14"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
-      <c r="G153" s="15"/>
-      <c r="H153" s="14"/>
+      <c r="D153" s="13">
+        <v>1</v>
+      </c>
+      <c r="E153" s="29"/>
+      <c r="F153" s="29"/>
+      <c r="G153" s="29"/>
+      <c r="H153" s="16"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A154" s="14">
-        <v>8</v>
-      </c>
+      <c r="A154" s="14"/>
       <c r="B154" s="14"/>
       <c r="C154" s="14"/>
-      <c r="D154" s="14"/>
-      <c r="E154" s="15"/>
-      <c r="F154" s="15"/>
-      <c r="G154" s="15"/>
-      <c r="H154" s="14"/>
+      <c r="D154" s="13">
+        <v>2</v>
+      </c>
+      <c r="E154" s="29"/>
+      <c r="F154" s="29"/>
+      <c r="G154" s="29"/>
+      <c r="H154" s="16"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A155" s="14">
-        <v>9</v>
-      </c>
+      <c r="A155" s="14"/>
       <c r="B155" s="14"/>
       <c r="C155" s="14"/>
-      <c r="D155" s="14"/>
-      <c r="E155" s="15"/>
-      <c r="F155" s="15"/>
-      <c r="G155" s="15"/>
-      <c r="H155" s="14"/>
+      <c r="D155" s="13">
+        <v>3</v>
+      </c>
+      <c r="E155" s="29"/>
+      <c r="F155" s="29"/>
+      <c r="G155" s="29"/>
+      <c r="H155" s="16"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A156" s="14">
-        <v>10</v>
-      </c>
+      <c r="A156" s="14"/>
       <c r="B156" s="14"/>
       <c r="C156" s="14"/>
-      <c r="D156" s="14"/>
-      <c r="E156" s="15"/>
-      <c r="F156" s="15"/>
-      <c r="G156" s="15"/>
-      <c r="H156" s="14"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="29"/>
+      <c r="F156" s="29"/>
+      <c r="G156" s="29"/>
+      <c r="H156" s="13"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A157" s="14">
-        <v>11</v>
-      </c>
+      <c r="A157" s="14"/>
       <c r="B157" s="14"/>
       <c r="C157" s="14"/>
-      <c r="D157" s="14"/>
-      <c r="E157" s="15"/>
-      <c r="F157" s="15"/>
-      <c r="G157" s="15"/>
-      <c r="H157" s="14"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="29"/>
+      <c r="F157" s="29"/>
+      <c r="G157" s="29"/>
+      <c r="H157" s="13"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A158" s="14">
-        <v>12</v>
-      </c>
+      <c r="A158" s="14"/>
       <c r="B158" s="14"/>
       <c r="C158" s="14"/>
-      <c r="D158" s="14"/>
-      <c r="E158" s="15"/>
-      <c r="F158" s="15"/>
-      <c r="G158" s="15"/>
-      <c r="H158" s="14"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="29"/>
+      <c r="F158" s="29"/>
+      <c r="G158" s="29"/>
+      <c r="H158" s="13"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A159" s="14">
-        <v>13</v>
-      </c>
+      <c r="A159" s="14"/>
       <c r="B159" s="14"/>
       <c r="C159" s="14"/>
       <c r="D159" s="14"/>
@@ -3814,10 +3912,14 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="14">
-        <v>14</v>
-      </c>
-      <c r="B160" s="14"/>
-      <c r="C160" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="B160" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="D160" s="14"/>
       <c r="E160" s="15"/>
       <c r="F160" s="15"/>
@@ -3825,9 +3927,7 @@
       <c r="H160" s="14"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="14">
-        <v>15</v>
-      </c>
+      <c r="A161" s="14"/>
       <c r="B161" s="14"/>
       <c r="C161" s="14"/>
       <c r="D161" s="14"/>
@@ -3838,7 +3938,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="14">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B162" s="14"/>
       <c r="C162" s="14"/>
@@ -3850,7 +3950,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="14">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B163" s="14"/>
       <c r="C163" s="14"/>
@@ -3862,7 +3962,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="14">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B164" s="14"/>
       <c r="C164" s="14"/>
@@ -3873,7 +3973,9 @@
       <c r="H164" s="14"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A165" s="14"/>
+      <c r="A165" s="14">
+        <v>10</v>
+      </c>
       <c r="B165" s="14"/>
       <c r="C165" s="14"/>
       <c r="D165" s="14"/>
@@ -3883,7 +3985,9 @@
       <c r="H165" s="14"/>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A166" s="14"/>
+      <c r="A166" s="14">
+        <v>11</v>
+      </c>
       <c r="B166" s="14"/>
       <c r="C166" s="14"/>
       <c r="D166" s="14"/>
@@ -3893,7 +3997,9 @@
       <c r="H166" s="14"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A167" s="14"/>
+      <c r="A167" s="14">
+        <v>12</v>
+      </c>
       <c r="B167" s="14"/>
       <c r="C167" s="14"/>
       <c r="D167" s="14"/>
@@ -3903,7 +4009,9 @@
       <c r="H167" s="14"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A168" s="14"/>
+      <c r="A168" s="14">
+        <v>13</v>
+      </c>
       <c r="B168" s="14"/>
       <c r="C168" s="14"/>
       <c r="D168" s="14"/>
@@ -3913,7 +4021,9 @@
       <c r="H168" s="14"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A169" s="14"/>
+      <c r="A169" s="14">
+        <v>14</v>
+      </c>
       <c r="B169" s="14"/>
       <c r="C169" s="14"/>
       <c r="D169" s="14"/>
@@ -3923,7 +4033,9 @@
       <c r="H169" s="14"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A170" s="14"/>
+      <c r="A170" s="14">
+        <v>15</v>
+      </c>
       <c r="B170" s="14"/>
       <c r="C170" s="14"/>
       <c r="D170" s="14"/>
@@ -3933,7 +4045,9 @@
       <c r="H170" s="14"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A171" s="14"/>
+      <c r="A171" s="14">
+        <v>16</v>
+      </c>
       <c r="B171" s="14"/>
       <c r="C171" s="14"/>
       <c r="D171" s="14"/>
@@ -3943,7 +4057,9 @@
       <c r="H171" s="14"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A172" s="14"/>
+      <c r="A172" s="14">
+        <v>17</v>
+      </c>
       <c r="B172" s="14"/>
       <c r="C172" s="14"/>
       <c r="D172" s="14"/>
@@ -3953,7 +4069,9 @@
       <c r="H172" s="14"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A173" s="14"/>
+      <c r="A173" s="14">
+        <v>18</v>
+      </c>
       <c r="B173" s="14"/>
       <c r="C173" s="14"/>
       <c r="D173" s="14"/>
@@ -3963,6 +4081,9 @@
       <c r="H173" s="14"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" s="14"/>
+      <c r="B174" s="14"/>
+      <c r="C174" s="14"/>
       <c r="D174" s="14"/>
       <c r="E174" s="15"/>
       <c r="F174" s="15"/>
@@ -3970,6 +4091,9 @@
       <c r="H174" s="14"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" s="14"/>
+      <c r="B175" s="14"/>
+      <c r="C175" s="14"/>
       <c r="D175" s="14"/>
       <c r="E175" s="15"/>
       <c r="F175" s="15"/>
@@ -3977,21 +4101,105 @@
       <c r="H175" s="14"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" s="14"/>
+      <c r="B176" s="14"/>
+      <c r="C176" s="14"/>
       <c r="D176" s="14"/>
       <c r="E176" s="15"/>
       <c r="F176" s="15"/>
       <c r="G176" s="15"/>
       <c r="H176" s="14"/>
     </row>
-    <row r="177" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" s="14"/>
+      <c r="B177" s="14"/>
+      <c r="C177" s="14"/>
       <c r="D177" s="14"/>
       <c r="E177" s="15"/>
       <c r="F177" s="15"/>
       <c r="G177" s="15"/>
       <c r="H177" s="14"/>
     </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" s="14"/>
+      <c r="B178" s="14"/>
+      <c r="C178" s="14"/>
+      <c r="D178" s="14"/>
+      <c r="E178" s="15"/>
+      <c r="F178" s="15"/>
+      <c r="G178" s="15"/>
+      <c r="H178" s="14"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" s="14"/>
+      <c r="B179" s="14"/>
+      <c r="C179" s="14"/>
+      <c r="D179" s="14"/>
+      <c r="E179" s="15"/>
+      <c r="F179" s="15"/>
+      <c r="G179" s="15"/>
+      <c r="H179" s="14"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" s="14"/>
+      <c r="B180" s="14"/>
+      <c r="C180" s="14"/>
+      <c r="D180" s="14"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="15"/>
+      <c r="G180" s="15"/>
+      <c r="H180" s="14"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" s="14"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="14"/>
+      <c r="D181" s="14"/>
+      <c r="E181" s="15"/>
+      <c r="F181" s="15"/>
+      <c r="G181" s="15"/>
+      <c r="H181" s="14"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" s="14"/>
+      <c r="B182" s="14"/>
+      <c r="C182" s="14"/>
+      <c r="D182" s="14"/>
+      <c r="E182" s="15"/>
+      <c r="F182" s="15"/>
+      <c r="G182" s="15"/>
+      <c r="H182" s="14"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D183" s="14"/>
+      <c r="E183" s="15"/>
+      <c r="F183" s="15"/>
+      <c r="G183" s="15"/>
+      <c r="H183" s="14"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D184" s="14"/>
+      <c r="E184" s="15"/>
+      <c r="F184" s="15"/>
+      <c r="G184" s="15"/>
+      <c r="H184" s="14"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D185" s="14"/>
+      <c r="E185" s="15"/>
+      <c r="F185" s="15"/>
+      <c r="G185" s="15"/>
+      <c r="H185" s="14"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D186" s="14"/>
+      <c r="E186" s="15"/>
+      <c r="F186" s="15"/>
+      <c r="G186" s="15"/>
+      <c r="H186" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H110:H121 H125:H129 H133:H134 H1:H61">
+  <conditionalFormatting sqref="H119:H130 H134:H138 H142:H143 H1:H61">
     <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4007,7 +4215,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62:H67">
+  <conditionalFormatting sqref="H62:H70">
     <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4015,7 +4223,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68:H73">
+  <conditionalFormatting sqref="H71:H79">
     <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4023,7 +4231,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H74:H79">
+  <conditionalFormatting sqref="H80:H88">
     <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4031,7 +4239,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H80:H85">
+  <conditionalFormatting sqref="H89:H94">
     <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4039,7 +4247,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H86:H91">
+  <conditionalFormatting sqref="H95:H100">
     <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4047,7 +4255,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H92:H97">
+  <conditionalFormatting sqref="H101:H106">
     <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4055,7 +4263,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H98:H103">
+  <conditionalFormatting sqref="H107:H112">
     <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4063,7 +4271,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H104:H109">
+  <conditionalFormatting sqref="H113:H118">
     <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4071,7 +4279,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H141:H146">
+  <conditionalFormatting sqref="H150:H155">
     <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4079,7 +4287,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H135:H140">
+  <conditionalFormatting sqref="H144:H149">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4087,7 +4295,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H122:H124">
+  <conditionalFormatting sqref="H131:H133">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4095,7 +4303,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H130:H132">
+  <conditionalFormatting sqref="H139:H141">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Revert "Completed Invoice layout version 1.0"
This reverts commit d77d1c5e648d13da5f6e113e4830a082c9025fac.
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{41D10F38-AA9E-4E5C-8F25-6BBB17517380}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{55225790-E440-4FF5-A4B0-DE1DBAFF81DC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{AFF0B8A1-9626-46B3-9A62-F42AFA134D79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="100">
   <si>
     <t>Test Case</t>
   </si>
@@ -325,48 +325,6 @@
   </si>
   <si>
     <t>Record should be displayed because the customer list grid will pull customers that do not yet have contacts associated with them.</t>
-  </si>
-  <si>
-    <t>Select an existing customer (Click on their name)</t>
-  </si>
-  <si>
-    <t>The Customer Details window should be displayed</t>
-  </si>
-  <si>
-    <t>Under the Address Section, click on the 'Add' link</t>
-  </si>
-  <si>
-    <t>A new Address entry should be displayed at the top of the section</t>
-  </si>
-  <si>
-    <t>Add a new Address that is different from the existing (Either Billing, Shipping or Other)</t>
-  </si>
-  <si>
-    <t>Screen should allow for entry of values</t>
-  </si>
-  <si>
-    <t>Bring up Customer Details screen again</t>
-  </si>
-  <si>
-    <t>The Customer Details window should display.  The new address should be displayed</t>
-  </si>
-  <si>
-    <t>Under the Contacts Section, click on the 'Add' link</t>
-  </si>
-  <si>
-    <t>A new Contacts entry should be displayed at the top of the section</t>
-  </si>
-  <si>
-    <t>Add a new Contact that is different from the existing (Either Primary, Secondary, or Other))</t>
-  </si>
-  <si>
-    <t>The Customer Details window should display.  The new contact should be displayed</t>
-  </si>
-  <si>
-    <t>Edit customer information (Name, etc.)</t>
-  </si>
-  <si>
-    <t>All fields should be editable except for the Setup Date and Setup By values.</t>
   </si>
 </sst>
 </file>
@@ -1250,10 +1208,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H186"/>
+  <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2392,253 +2350,227 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="13">
         <v>1</v>
       </c>
-      <c r="E65" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F65" s="29" t="s">
-        <v>44</v>
-      </c>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
       <c r="G65" s="29"/>
       <c r="H65" s="16"/>
     </row>
-    <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="13">
         <v>2</v>
       </c>
-      <c r="E66" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="F66" s="29" t="s">
-        <v>101</v>
-      </c>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
       <c r="G66" s="29"/>
       <c r="H66" s="16"/>
     </row>
-    <row r="67" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
       <c r="D67" s="13">
         <v>3</v>
       </c>
-      <c r="E67" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="F67" s="29" t="s">
-        <v>103</v>
-      </c>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
       <c r="G67" s="29"/>
       <c r="H67" s="16"/>
     </row>
-    <row r="68" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="13">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="30"/>
+      <c r="E68" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>11</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="27"/>
+      <c r="E69" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="16"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="22"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E68" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F68" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="G68" s="29"/>
-      <c r="H68" s="16"/>
-    </row>
-    <row r="69" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="13">
+      <c r="G70" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E69" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="F69" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="G69" s="29"/>
-      <c r="H69" s="16"/>
-    </row>
-    <row r="70" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="13">
-        <v>6</v>
-      </c>
-      <c r="E70" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F70" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="G70" s="29"/>
-      <c r="H70" s="16"/>
+      <c r="H70" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="30" t="s">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="13">
+        <v>1</v>
+      </c>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="16"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="13">
+        <v>2</v>
+      </c>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="16"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="13">
+        <v>3</v>
+      </c>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="16"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="30" t="s">
+      <c r="B74" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D71" s="30"/>
-      <c r="E71" s="31" t="s">
+      <c r="D74" s="30"/>
+      <c r="E74" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A72" s="6">
-        <v>11</v>
-      </c>
-      <c r="B72" s="6" t="s">
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>12</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" s="27"/>
-      <c r="E72" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F72" s="28"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="16"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="22"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F73" s="11" t="s">
+      <c r="C75" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75" s="27"/>
+      <c r="E75" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="16"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G73" s="11" t="s">
+      <c r="G76" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H73" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="13">
-        <v>1</v>
-      </c>
-      <c r="E74" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F74" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="G74" s="29"/>
-      <c r="H74" s="16"/>
-    </row>
-    <row r="75" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="13">
-        <v>2</v>
-      </c>
-      <c r="E75" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="F75" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="G75" s="29"/>
-      <c r="H75" s="16"/>
-    </row>
-    <row r="76" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="13">
-        <v>3</v>
-      </c>
-      <c r="E76" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="F76" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="G76" s="29"/>
-      <c r="H76" s="16"/>
-    </row>
-    <row r="77" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="H76" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
       <c r="D77" s="13">
-        <v>4</v>
-      </c>
-      <c r="E77" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F77" s="29" t="s">
-        <v>105</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
       <c r="G77" s="29"/>
       <c r="H77" s="16"/>
     </row>
-    <row r="78" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
       <c r="D78" s="13">
-        <v>5</v>
-      </c>
-      <c r="E78" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="F78" s="29" t="s">
-        <v>94</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
       <c r="G78" s="29"/>
       <c r="H78" s="16"/>
     </row>
-    <row r="79" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="D79" s="13">
-        <v>6</v>
-      </c>
-      <c r="E79" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F79" s="29" t="s">
-        <v>111</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
       <c r="G79" s="29"/>
       <c r="H79" s="16"/>
     </row>
@@ -2664,7 +2596,7 @@
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>7</v>
@@ -2674,7 +2606,7 @@
       </c>
       <c r="D81" s="27"/>
       <c r="E81" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F81" s="28"/>
       <c r="G81" s="28"/>
@@ -2700,581 +2632,595 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
       <c r="D83" s="13">
         <v>1</v>
       </c>
-      <c r="E83" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F83" s="29" t="s">
-        <v>44</v>
-      </c>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
       <c r="G83" s="29"/>
       <c r="H83" s="16"/>
     </row>
-    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
       <c r="D84" s="13">
         <v>2</v>
       </c>
-      <c r="E84" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="F84" s="29" t="s">
-        <v>101</v>
-      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
       <c r="G84" s="29"/>
       <c r="H84" s="16"/>
     </row>
-    <row r="85" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
       <c r="D85" s="13">
         <v>3</v>
       </c>
-      <c r="E85" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="F85" s="29" t="s">
-        <v>113</v>
-      </c>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
       <c r="G85" s="29"/>
       <c r="H85" s="16"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="14"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="13">
+      <c r="A86" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="30"/>
+      <c r="E86" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F86" s="31"/>
+      <c r="G86" s="31"/>
+      <c r="H86" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>14</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D87" s="27"/>
+      <c r="E87" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F87" s="28"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="16"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="22"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F88" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
-      <c r="G86" s="29"/>
-      <c r="H86" s="16"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="14"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="13">
+      <c r="G88" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="16"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="14"/>
-      <c r="B88" s="14"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="29"/>
-      <c r="G88" s="29"/>
-      <c r="H88" s="16"/>
+      <c r="H88" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="30" t="s">
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="13">
+        <v>1</v>
+      </c>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="29"/>
+      <c r="H89" s="16"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="13">
+        <v>2</v>
+      </c>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="16"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="13">
+        <v>3</v>
+      </c>
+      <c r="E91" s="29"/>
+      <c r="F91" s="29"/>
+      <c r="G91" s="29"/>
+      <c r="H91" s="16"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="30" t="s">
+      <c r="B92" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D89" s="30"/>
-      <c r="E89" s="31" t="s">
+      <c r="D92" s="30"/>
+      <c r="E92" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F89" s="31"/>
-      <c r="G89" s="31"/>
-      <c r="H89" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="6">
-        <v>13</v>
-      </c>
-      <c r="B90" s="6" t="s">
+      <c r="F92" s="31"/>
+      <c r="G92" s="31"/>
+      <c r="H92" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>15</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C90" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D90" s="27"/>
-      <c r="E90" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F90" s="28"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="16"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="22"/>
-      <c r="B91" s="22"/>
-      <c r="C91" s="22"/>
-      <c r="D91" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E91" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F91" s="11" t="s">
+      <c r="C93" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D93" s="27"/>
+      <c r="E93" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F93" s="28"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="16"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="22"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F94" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G91" s="11" t="s">
+      <c r="G94" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H91" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="13">
-        <v>1</v>
-      </c>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
-      <c r="G92" s="29"/>
-      <c r="H92" s="16"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="14"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="13">
-        <v>2</v>
-      </c>
-      <c r="E93" s="29"/>
-      <c r="F93" s="29"/>
-      <c r="G93" s="29"/>
-      <c r="H93" s="16"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="14"/>
-      <c r="B94" s="14"/>
-      <c r="C94" s="14"/>
-      <c r="D94" s="13">
-        <v>3</v>
-      </c>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="16"/>
+      <c r="H94" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="30" t="s">
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="13">
+        <v>1</v>
+      </c>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
+      <c r="H95" s="16"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="13">
+        <v>2</v>
+      </c>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="16"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="13">
+        <v>3</v>
+      </c>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="16"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B95" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="30" t="s">
+      <c r="B98" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D95" s="30"/>
-      <c r="E95" s="31" t="s">
+      <c r="D98" s="30"/>
+      <c r="E98" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F95" s="31"/>
-      <c r="G95" s="31"/>
-      <c r="H95" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="6">
-        <v>14</v>
-      </c>
-      <c r="B96" s="6" t="s">
+      <c r="F98" s="31"/>
+      <c r="G98" s="31"/>
+      <c r="H98" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>16</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D96" s="27"/>
-      <c r="E96" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F96" s="28"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="16"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="22"/>
-      <c r="B97" s="22"/>
-      <c r="C97" s="22"/>
-      <c r="D97" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E97" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F97" s="11" t="s">
+      <c r="C99" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D99" s="27"/>
+      <c r="E99" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F99" s="28"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="16"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="22"/>
+      <c r="B100" s="22"/>
+      <c r="C100" s="22"/>
+      <c r="D100" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F100" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G97" s="11" t="s">
+      <c r="G100" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H97" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="14"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="13">
-        <v>1</v>
-      </c>
-      <c r="E98" s="29"/>
-      <c r="F98" s="29"/>
-      <c r="G98" s="29"/>
-      <c r="H98" s="16"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="14"/>
-      <c r="B99" s="14"/>
-      <c r="C99" s="14"/>
-      <c r="D99" s="13">
-        <v>2</v>
-      </c>
-      <c r="E99" s="29"/>
-      <c r="F99" s="29"/>
-      <c r="G99" s="29"/>
-      <c r="H99" s="16"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="14"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="13">
-        <v>3</v>
-      </c>
-      <c r="E100" s="29"/>
-      <c r="F100" s="29"/>
-      <c r="G100" s="29"/>
-      <c r="H100" s="16"/>
+      <c r="H100" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="30" t="s">
+      <c r="A101" s="14"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="13">
+        <v>1</v>
+      </c>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="16"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="13">
+        <v>2</v>
+      </c>
+      <c r="E102" s="29"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="29"/>
+      <c r="H102" s="16"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="13">
+        <v>3</v>
+      </c>
+      <c r="E103" s="29"/>
+      <c r="F103" s="29"/>
+      <c r="G103" s="29"/>
+      <c r="H103" s="16"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B101" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="30" t="s">
+      <c r="B104" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D101" s="30"/>
-      <c r="E101" s="31" t="s">
+      <c r="D104" s="30"/>
+      <c r="E104" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F101" s="31"/>
-      <c r="G101" s="31"/>
-      <c r="H101" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A102" s="6">
-        <v>15</v>
-      </c>
-      <c r="B102" s="6" t="s">
+      <c r="F104" s="31"/>
+      <c r="G104" s="31"/>
+      <c r="H104" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A105" s="6">
+        <v>17</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D102" s="27"/>
-      <c r="E102" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F102" s="28"/>
-      <c r="G102" s="28"/>
-      <c r="H102" s="16"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="22"/>
-      <c r="B103" s="22"/>
-      <c r="C103" s="22"/>
-      <c r="D103" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F103" s="11" t="s">
+      <c r="C105" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D105" s="27"/>
+      <c r="E105" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F105" s="28"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="16"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="22"/>
+      <c r="B106" s="22"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E106" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F106" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G103" s="11" t="s">
+      <c r="G106" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H103" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="14"/>
-      <c r="D104" s="13">
-        <v>1</v>
-      </c>
-      <c r="E104" s="29"/>
-      <c r="F104" s="29"/>
-      <c r="G104" s="29"/>
-      <c r="H104" s="16"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="13">
-        <v>2</v>
-      </c>
-      <c r="E105" s="29"/>
-      <c r="F105" s="29"/>
-      <c r="G105" s="29"/>
-      <c r="H105" s="16"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="13">
-        <v>3</v>
-      </c>
-      <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
-      <c r="G106" s="29"/>
-      <c r="H106" s="16"/>
+      <c r="H106" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="30" t="s">
+      <c r="A107" s="14"/>
+      <c r="B107" s="14"/>
+      <c r="C107" s="14"/>
+      <c r="D107" s="13">
+        <v>1</v>
+      </c>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="16"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="14"/>
+      <c r="D108" s="13">
+        <v>2</v>
+      </c>
+      <c r="E108" s="29"/>
+      <c r="F108" s="29"/>
+      <c r="G108" s="29"/>
+      <c r="H108" s="16"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="14"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="14"/>
+      <c r="D109" s="13">
+        <v>3</v>
+      </c>
+      <c r="E109" s="29"/>
+      <c r="F109" s="29"/>
+      <c r="G109" s="29"/>
+      <c r="H109" s="16"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B107" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C107" s="30" t="s">
+      <c r="B110" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D107" s="30"/>
-      <c r="E107" s="31" t="s">
+      <c r="D110" s="25"/>
+      <c r="E110" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F107" s="31"/>
-      <c r="G107" s="31"/>
-      <c r="H107" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A108" s="6">
-        <v>16</v>
-      </c>
-      <c r="B108" s="6" t="s">
+      <c r="F110" s="26"/>
+      <c r="G110" s="26"/>
+      <c r="H110" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A111" s="6">
+        <v>18</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C108" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D108" s="27"/>
-      <c r="E108" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F108" s="28"/>
-      <c r="G108" s="28"/>
-      <c r="H108" s="16"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="22"/>
-      <c r="B109" s="22"/>
-      <c r="C109" s="22"/>
-      <c r="D109" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E109" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F109" s="11" t="s">
+      <c r="C111" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D111" s="27"/>
+      <c r="E111" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F111" s="28"/>
+      <c r="G111" s="28"/>
+      <c r="H111" s="16"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="22"/>
+      <c r="B112" s="22"/>
+      <c r="C112" s="22"/>
+      <c r="D112" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F112" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G109" s="11" t="s">
+      <c r="G112" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H109" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="14"/>
-      <c r="D110" s="13">
-        <v>1</v>
-      </c>
-      <c r="E110" s="29"/>
-      <c r="F110" s="29"/>
-      <c r="G110" s="29"/>
-      <c r="H110" s="16"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="14"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="13">
-        <v>2</v>
-      </c>
-      <c r="E111" s="29"/>
-      <c r="F111" s="29"/>
-      <c r="G111" s="29"/>
-      <c r="H111" s="16"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="14"/>
-      <c r="D112" s="13">
-        <v>3</v>
-      </c>
-      <c r="E112" s="29"/>
-      <c r="F112" s="29"/>
-      <c r="G112" s="29"/>
-      <c r="H112" s="16"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B113" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C113" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D113" s="30"/>
-      <c r="E113" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F113" s="31"/>
-      <c r="G113" s="31"/>
-      <c r="H113" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A114" s="6">
-        <v>17</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D114" s="27"/>
-      <c r="E114" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F114" s="28"/>
-      <c r="G114" s="28"/>
+      <c r="H112" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="13">
+        <v>1</v>
+      </c>
+      <c r="E113" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F113" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G113" s="23"/>
+      <c r="H113" s="16"/>
+    </row>
+    <row r="114" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="14"/>
+      <c r="D114" s="13">
+        <v>2</v>
+      </c>
+      <c r="E114" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F114" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G114" s="23"/>
       <c r="H114" s="16"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="22"/>
-      <c r="B115" s="22"/>
-      <c r="C115" s="22"/>
-      <c r="D115" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E115" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F115" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G115" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H115" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="14"/>
+      <c r="D115" s="13">
+        <v>3</v>
+      </c>
+      <c r="E115" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F115" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G115" s="23"/>
+      <c r="H115" s="16"/>
+    </row>
+    <row r="116" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A116" s="14"/>
       <c r="B116" s="14"/>
       <c r="C116" s="14"/>
       <c r="D116" s="13">
-        <v>1</v>
-      </c>
-      <c r="E116" s="29"/>
-      <c r="F116" s="29"/>
-      <c r="G116" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="E116" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F116" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G116" s="23"/>
       <c r="H116" s="16"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A117" s="14"/>
       <c r="B117" s="14"/>
       <c r="C117" s="14"/>
       <c r="D117" s="13">
-        <v>2</v>
-      </c>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
+        <v>4</v>
+      </c>
+      <c r="E117" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F117" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G117" s="23"/>
       <c r="H117" s="16"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A118" s="14"/>
       <c r="B118" s="14"/>
       <c r="C118" s="14"/>
       <c r="D118" s="13">
-        <v>3</v>
-      </c>
-      <c r="E118" s="29"/>
-      <c r="F118" s="29"/>
-      <c r="G118" s="29"/>
+        <v>5</v>
+      </c>
+      <c r="E118" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F118" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G118" s="23"/>
       <c r="H118" s="16"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="25" t="s">
+      <c r="A119" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B119" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="25" t="s">
+      <c r="B119" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D119" s="25"/>
-      <c r="E119" s="26" t="s">
+      <c r="D119" s="30"/>
+      <c r="E119" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F119" s="26"/>
-      <c r="G119" s="26"/>
+      <c r="F119" s="31"/>
+      <c r="G119" s="31"/>
       <c r="H119" s="33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>7</v>
@@ -3284,7 +3230,7 @@
       </c>
       <c r="D120" s="27"/>
       <c r="E120" s="7" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F120" s="28"/>
       <c r="G120" s="28"/>
@@ -3358,550 +3304,506 @@
       <c r="G124" s="23"/>
       <c r="H124" s="16"/>
     </row>
-    <row r="125" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A125" s="14"/>
       <c r="B125" s="14"/>
       <c r="C125" s="14"/>
       <c r="D125" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E125" s="29" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="F125" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="G125" s="23"/>
+        <v>50</v>
+      </c>
+      <c r="G125" s="29"/>
       <c r="H125" s="16"/>
     </row>
-    <row r="126" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A126" s="14"/>
       <c r="B126" s="14"/>
       <c r="C126" s="14"/>
       <c r="D126" s="13">
+        <v>5</v>
+      </c>
+      <c r="E126" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F126" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G126" s="29"/>
+      <c r="H126" s="16"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D127" s="30"/>
+      <c r="E127" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F127" s="31"/>
+      <c r="G127" s="31"/>
+      <c r="H127" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A128" s="6">
+        <v>20</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D128" s="27"/>
+      <c r="E128" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F128" s="28"/>
+      <c r="G128" s="28"/>
+      <c r="H128" s="16"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" s="22"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="22"/>
+      <c r="D129" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E129" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F129" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E126" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="F126" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="G126" s="23"/>
-      <c r="H126" s="16"/>
-    </row>
-    <row r="127" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A127" s="14"/>
-      <c r="B127" s="14"/>
-      <c r="C127" s="14"/>
-      <c r="D127" s="13">
+      <c r="G129" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E127" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="F127" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="G127" s="23"/>
-      <c r="H127" s="16"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B128" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C128" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D128" s="30"/>
-      <c r="E128" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F128" s="31"/>
-      <c r="G128" s="31"/>
-      <c r="H128" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A129" s="6">
-        <v>19</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D129" s="27"/>
-      <c r="E129" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F129" s="28"/>
-      <c r="G129" s="28"/>
-      <c r="H129" s="16"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="22"/>
-      <c r="B130" s="22"/>
-      <c r="C130" s="22"/>
-      <c r="D130" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E130" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F130" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G130" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H130" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="H129" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A130" s="14"/>
+      <c r="B130" s="14"/>
+      <c r="C130" s="14"/>
+      <c r="D130" s="13">
+        <v>1</v>
+      </c>
+      <c r="E130" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F130" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G130" s="23"/>
+      <c r="H130" s="16"/>
+    </row>
+    <row r="131" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" s="14"/>
       <c r="B131" s="14"/>
       <c r="C131" s="14"/>
       <c r="D131" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E131" s="29" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="F131" s="29" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="G131" s="23"/>
       <c r="H131" s="16"/>
     </row>
-    <row r="132" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A132" s="14"/>
       <c r="B132" s="14"/>
       <c r="C132" s="14"/>
       <c r="D132" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E132" s="29" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F132" s="29" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="G132" s="23"/>
       <c r="H132" s="16"/>
     </row>
-    <row r="133" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A133" s="14"/>
       <c r="B133" s="14"/>
       <c r="C133" s="14"/>
       <c r="D133" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E133" s="29" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="F133" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G133" s="23"/>
+        <v>56</v>
+      </c>
+      <c r="G133" s="29"/>
       <c r="H133" s="16"/>
     </row>
-    <row r="134" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A134" s="14"/>
       <c r="B134" s="14"/>
       <c r="C134" s="14"/>
       <c r="D134" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="F134" s="29" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G134" s="29"/>
       <c r="H134" s="16"/>
     </row>
-    <row r="135" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A135" s="14"/>
-      <c r="B135" s="14"/>
-      <c r="C135" s="14"/>
-      <c r="D135" s="13">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D135" s="30"/>
+      <c r="E135" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F135" s="31"/>
+      <c r="G135" s="31"/>
+      <c r="H135" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A136" s="6">
+        <v>21</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D136" s="27"/>
+      <c r="E136" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F136" s="28"/>
+      <c r="G136" s="28"/>
+      <c r="H136" s="16"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="22"/>
+      <c r="B137" s="22"/>
+      <c r="C137" s="22"/>
+      <c r="D137" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E137" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F137" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G137" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E135" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F135" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="G135" s="29"/>
-      <c r="H135" s="16"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B136" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C136" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D136" s="30"/>
-      <c r="E136" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F136" s="31"/>
-      <c r="G136" s="31"/>
-      <c r="H136" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A137" s="6">
-        <v>20</v>
-      </c>
-      <c r="B137" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D137" s="27"/>
-      <c r="E137" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F137" s="28"/>
-      <c r="G137" s="28"/>
-      <c r="H137" s="16"/>
+      <c r="H137" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="22"/>
-      <c r="B138" s="22"/>
-      <c r="C138" s="22"/>
-      <c r="D138" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E138" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F138" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G138" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H138" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A138" s="14"/>
+      <c r="B138" s="14"/>
+      <c r="C138" s="14"/>
+      <c r="D138" s="13">
+        <v>1</v>
+      </c>
+      <c r="E138" s="29"/>
+      <c r="F138" s="29"/>
+      <c r="G138" s="29"/>
+      <c r="H138" s="16"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="14"/>
       <c r="B139" s="14"/>
       <c r="C139" s="14"/>
       <c r="D139" s="13">
-        <v>1</v>
-      </c>
-      <c r="E139" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F139" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G139" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="E139" s="29"/>
+      <c r="F139" s="29"/>
+      <c r="G139" s="29"/>
       <c r="H139" s="16"/>
     </row>
-    <row r="140" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="14"/>
       <c r="B140" s="14"/>
       <c r="C140" s="14"/>
       <c r="D140" s="13">
-        <v>2</v>
-      </c>
-      <c r="E140" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F140" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G140" s="23"/>
+        <v>3</v>
+      </c>
+      <c r="E140" s="29"/>
+      <c r="F140" s="29"/>
+      <c r="G140" s="29"/>
       <c r="H140" s="16"/>
     </row>
-    <row r="141" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A141" s="14"/>
-      <c r="B141" s="14"/>
-      <c r="C141" s="14"/>
-      <c r="D141" s="13">
-        <v>3</v>
-      </c>
-      <c r="E141" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F141" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G141" s="23"/>
-      <c r="H141" s="16"/>
-    </row>
-    <row r="142" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A142" s="14"/>
-      <c r="B142" s="14"/>
-      <c r="C142" s="14"/>
-      <c r="D142" s="13">
-        <v>2</v>
-      </c>
-      <c r="E142" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F142" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="G142" s="29"/>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D141" s="30"/>
+      <c r="E141" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F141" s="31"/>
+      <c r="G141" s="31"/>
+      <c r="H141" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A142" s="6">
+        <v>22</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D142" s="27"/>
+      <c r="E142" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F142" s="28"/>
+      <c r="G142" s="28"/>
       <c r="H142" s="16"/>
     </row>
-    <row r="143" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A143" s="14"/>
-      <c r="B143" s="14"/>
-      <c r="C143" s="14"/>
-      <c r="D143" s="13">
-        <v>3</v>
-      </c>
-      <c r="E143" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="F143" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="G143" s="29"/>
-      <c r="H143" s="16"/>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" s="22"/>
+      <c r="B143" s="22"/>
+      <c r="C143" s="22"/>
+      <c r="D143" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E143" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F143" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G143" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H143" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B144" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C144" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D144" s="30"/>
-      <c r="E144" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F144" s="31"/>
-      <c r="G144" s="31"/>
-      <c r="H144" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A145" s="6">
-        <v>21</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C145" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D145" s="27"/>
-      <c r="E145" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F145" s="28"/>
-      <c r="G145" s="28"/>
+      <c r="A144" s="14"/>
+      <c r="B144" s="14"/>
+      <c r="C144" s="14"/>
+      <c r="D144" s="13">
+        <v>1</v>
+      </c>
+      <c r="E144" s="29"/>
+      <c r="F144" s="29"/>
+      <c r="G144" s="29"/>
+      <c r="H144" s="16"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" s="14"/>
+      <c r="B145" s="14"/>
+      <c r="C145" s="14"/>
+      <c r="D145" s="13">
+        <v>2</v>
+      </c>
+      <c r="E145" s="29"/>
+      <c r="F145" s="29"/>
+      <c r="G145" s="29"/>
       <c r="H145" s="16"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A146" s="22"/>
-      <c r="B146" s="22"/>
-      <c r="C146" s="22"/>
-      <c r="D146" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E146" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F146" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G146" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H146" s="34" t="s">
-        <v>6</v>
-      </c>
+      <c r="A146" s="14"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="14"/>
+      <c r="D146" s="13">
+        <v>3</v>
+      </c>
+      <c r="E146" s="29"/>
+      <c r="F146" s="29"/>
+      <c r="G146" s="29"/>
+      <c r="H146" s="16"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="14"/>
       <c r="B147" s="14"/>
       <c r="C147" s="14"/>
-      <c r="D147" s="13">
-        <v>1</v>
-      </c>
+      <c r="D147" s="13"/>
       <c r="E147" s="29"/>
       <c r="F147" s="29"/>
       <c r="G147" s="29"/>
-      <c r="H147" s="16"/>
+      <c r="H147" s="13"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="14"/>
       <c r="B148" s="14"/>
       <c r="C148" s="14"/>
-      <c r="D148" s="13">
-        <v>2</v>
-      </c>
+      <c r="D148" s="13"/>
       <c r="E148" s="29"/>
       <c r="F148" s="29"/>
       <c r="G148" s="29"/>
-      <c r="H148" s="16"/>
+      <c r="H148" s="13"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="14"/>
       <c r="B149" s="14"/>
       <c r="C149" s="14"/>
-      <c r="D149" s="13">
-        <v>3</v>
-      </c>
+      <c r="D149" s="13"/>
       <c r="E149" s="29"/>
       <c r="F149" s="29"/>
       <c r="G149" s="29"/>
-      <c r="H149" s="16"/>
+      <c r="H149" s="13"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A150" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B150" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C150" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D150" s="30"/>
-      <c r="E150" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F150" s="31"/>
-      <c r="G150" s="31"/>
-      <c r="H150" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A151" s="6">
-        <v>22</v>
-      </c>
-      <c r="B151" s="6" t="s">
+      <c r="A150" s="14"/>
+      <c r="B150" s="14"/>
+      <c r="C150" s="14"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="15"/>
+      <c r="F150" s="15"/>
+      <c r="G150" s="15"/>
+      <c r="H150" s="14"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="14">
+        <v>5</v>
+      </c>
+      <c r="B151" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C151" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D151" s="27"/>
-      <c r="E151" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F151" s="28"/>
-      <c r="G151" s="28"/>
-      <c r="H151" s="16"/>
+      <c r="C151" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D151" s="14"/>
+      <c r="E151" s="15"/>
+      <c r="F151" s="15"/>
+      <c r="G151" s="15"/>
+      <c r="H151" s="14"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A152" s="22"/>
-      <c r="B152" s="22"/>
-      <c r="C152" s="22"/>
-      <c r="D152" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E152" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F152" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G152" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H152" s="34" t="s">
-        <v>6</v>
-      </c>
+      <c r="A152" s="14"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="14"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="15"/>
+      <c r="F152" s="15"/>
+      <c r="G152" s="15"/>
+      <c r="H152" s="14"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A153" s="14"/>
+      <c r="A153" s="14">
+        <v>7</v>
+      </c>
       <c r="B153" s="14"/>
       <c r="C153" s="14"/>
-      <c r="D153" s="13">
-        <v>1</v>
-      </c>
-      <c r="E153" s="29"/>
-      <c r="F153" s="29"/>
-      <c r="G153" s="29"/>
-      <c r="H153" s="16"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
+      <c r="G153" s="15"/>
+      <c r="H153" s="14"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A154" s="14"/>
+      <c r="A154" s="14">
+        <v>8</v>
+      </c>
       <c r="B154" s="14"/>
       <c r="C154" s="14"/>
-      <c r="D154" s="13">
-        <v>2</v>
-      </c>
-      <c r="E154" s="29"/>
-      <c r="F154" s="29"/>
-      <c r="G154" s="29"/>
-      <c r="H154" s="16"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="15"/>
+      <c r="F154" s="15"/>
+      <c r="G154" s="15"/>
+      <c r="H154" s="14"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A155" s="14"/>
+      <c r="A155" s="14">
+        <v>9</v>
+      </c>
       <c r="B155" s="14"/>
       <c r="C155" s="14"/>
-      <c r="D155" s="13">
-        <v>3</v>
-      </c>
-      <c r="E155" s="29"/>
-      <c r="F155" s="29"/>
-      <c r="G155" s="29"/>
-      <c r="H155" s="16"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="15"/>
+      <c r="F155" s="15"/>
+      <c r="G155" s="15"/>
+      <c r="H155" s="14"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A156" s="14"/>
+      <c r="A156" s="14">
+        <v>10</v>
+      </c>
       <c r="B156" s="14"/>
       <c r="C156" s="14"/>
-      <c r="D156" s="13"/>
-      <c r="E156" s="29"/>
-      <c r="F156" s="29"/>
-      <c r="G156" s="29"/>
-      <c r="H156" s="13"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="15"/>
+      <c r="F156" s="15"/>
+      <c r="G156" s="15"/>
+      <c r="H156" s="14"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A157" s="14"/>
+      <c r="A157" s="14">
+        <v>11</v>
+      </c>
       <c r="B157" s="14"/>
       <c r="C157" s="14"/>
-      <c r="D157" s="13"/>
-      <c r="E157" s="29"/>
-      <c r="F157" s="29"/>
-      <c r="G157" s="29"/>
-      <c r="H157" s="13"/>
+      <c r="D157" s="14"/>
+      <c r="E157" s="15"/>
+      <c r="F157" s="15"/>
+      <c r="G157" s="15"/>
+      <c r="H157" s="14"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A158" s="14"/>
+      <c r="A158" s="14">
+        <v>12</v>
+      </c>
       <c r="B158" s="14"/>
       <c r="C158" s="14"/>
-      <c r="D158" s="13"/>
-      <c r="E158" s="29"/>
-      <c r="F158" s="29"/>
-      <c r="G158" s="29"/>
-      <c r="H158" s="13"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="15"/>
+      <c r="F158" s="15"/>
+      <c r="G158" s="15"/>
+      <c r="H158" s="14"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A159" s="14"/>
+      <c r="A159" s="14">
+        <v>13</v>
+      </c>
       <c r="B159" s="14"/>
       <c r="C159" s="14"/>
       <c r="D159" s="14"/>
@@ -3912,14 +3814,10 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="14">
-        <v>5</v>
-      </c>
-      <c r="B160" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C160" s="14" t="s">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B160" s="14"/>
+      <c r="C160" s="14"/>
       <c r="D160" s="14"/>
       <c r="E160" s="15"/>
       <c r="F160" s="15"/>
@@ -3927,7 +3825,9 @@
       <c r="H160" s="14"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="14"/>
+      <c r="A161" s="14">
+        <v>15</v>
+      </c>
       <c r="B161" s="14"/>
       <c r="C161" s="14"/>
       <c r="D161" s="14"/>
@@ -3938,7 +3838,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="14">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B162" s="14"/>
       <c r="C162" s="14"/>
@@ -3950,7 +3850,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="14">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B163" s="14"/>
       <c r="C163" s="14"/>
@@ -3962,7 +3862,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="14">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B164" s="14"/>
       <c r="C164" s="14"/>
@@ -3973,9 +3873,7 @@
       <c r="H164" s="14"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A165" s="14">
-        <v>10</v>
-      </c>
+      <c r="A165" s="14"/>
       <c r="B165" s="14"/>
       <c r="C165" s="14"/>
       <c r="D165" s="14"/>
@@ -3985,9 +3883,7 @@
       <c r="H165" s="14"/>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A166" s="14">
-        <v>11</v>
-      </c>
+      <c r="A166" s="14"/>
       <c r="B166" s="14"/>
       <c r="C166" s="14"/>
       <c r="D166" s="14"/>
@@ -3997,9 +3893,7 @@
       <c r="H166" s="14"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A167" s="14">
-        <v>12</v>
-      </c>
+      <c r="A167" s="14"/>
       <c r="B167" s="14"/>
       <c r="C167" s="14"/>
       <c r="D167" s="14"/>
@@ -4009,9 +3903,7 @@
       <c r="H167" s="14"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A168" s="14">
-        <v>13</v>
-      </c>
+      <c r="A168" s="14"/>
       <c r="B168" s="14"/>
       <c r="C168" s="14"/>
       <c r="D168" s="14"/>
@@ -4021,9 +3913,7 @@
       <c r="H168" s="14"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A169" s="14">
-        <v>14</v>
-      </c>
+      <c r="A169" s="14"/>
       <c r="B169" s="14"/>
       <c r="C169" s="14"/>
       <c r="D169" s="14"/>
@@ -4033,9 +3923,7 @@
       <c r="H169" s="14"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A170" s="14">
-        <v>15</v>
-      </c>
+      <c r="A170" s="14"/>
       <c r="B170" s="14"/>
       <c r="C170" s="14"/>
       <c r="D170" s="14"/>
@@ -4045,9 +3933,7 @@
       <c r="H170" s="14"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A171" s="14">
-        <v>16</v>
-      </c>
+      <c r="A171" s="14"/>
       <c r="B171" s="14"/>
       <c r="C171" s="14"/>
       <c r="D171" s="14"/>
@@ -4057,9 +3943,7 @@
       <c r="H171" s="14"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A172" s="14">
-        <v>17</v>
-      </c>
+      <c r="A172" s="14"/>
       <c r="B172" s="14"/>
       <c r="C172" s="14"/>
       <c r="D172" s="14"/>
@@ -4069,9 +3953,7 @@
       <c r="H172" s="14"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A173" s="14">
-        <v>18</v>
-      </c>
+      <c r="A173" s="14"/>
       <c r="B173" s="14"/>
       <c r="C173" s="14"/>
       <c r="D173" s="14"/>
@@ -4081,9 +3963,6 @@
       <c r="H173" s="14"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A174" s="14"/>
-      <c r="B174" s="14"/>
-      <c r="C174" s="14"/>
       <c r="D174" s="14"/>
       <c r="E174" s="15"/>
       <c r="F174" s="15"/>
@@ -4091,9 +3970,6 @@
       <c r="H174" s="14"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A175" s="14"/>
-      <c r="B175" s="14"/>
-      <c r="C175" s="14"/>
       <c r="D175" s="14"/>
       <c r="E175" s="15"/>
       <c r="F175" s="15"/>
@@ -4101,105 +3977,21 @@
       <c r="H175" s="14"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A176" s="14"/>
-      <c r="B176" s="14"/>
-      <c r="C176" s="14"/>
       <c r="D176" s="14"/>
       <c r="E176" s="15"/>
       <c r="F176" s="15"/>
       <c r="G176" s="15"/>
       <c r="H176" s="14"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A177" s="14"/>
-      <c r="B177" s="14"/>
-      <c r="C177" s="14"/>
+    <row r="177" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D177" s="14"/>
       <c r="E177" s="15"/>
       <c r="F177" s="15"/>
       <c r="G177" s="15"/>
       <c r="H177" s="14"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A178" s="14"/>
-      <c r="B178" s="14"/>
-      <c r="C178" s="14"/>
-      <c r="D178" s="14"/>
-      <c r="E178" s="15"/>
-      <c r="F178" s="15"/>
-      <c r="G178" s="15"/>
-      <c r="H178" s="14"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A179" s="14"/>
-      <c r="B179" s="14"/>
-      <c r="C179" s="14"/>
-      <c r="D179" s="14"/>
-      <c r="E179" s="15"/>
-      <c r="F179" s="15"/>
-      <c r="G179" s="15"/>
-      <c r="H179" s="14"/>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A180" s="14"/>
-      <c r="B180" s="14"/>
-      <c r="C180" s="14"/>
-      <c r="D180" s="14"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="15"/>
-      <c r="G180" s="15"/>
-      <c r="H180" s="14"/>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A181" s="14"/>
-      <c r="B181" s="14"/>
-      <c r="C181" s="14"/>
-      <c r="D181" s="14"/>
-      <c r="E181" s="15"/>
-      <c r="F181" s="15"/>
-      <c r="G181" s="15"/>
-      <c r="H181" s="14"/>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A182" s="14"/>
-      <c r="B182" s="14"/>
-      <c r="C182" s="14"/>
-      <c r="D182" s="14"/>
-      <c r="E182" s="15"/>
-      <c r="F182" s="15"/>
-      <c r="G182" s="15"/>
-      <c r="H182" s="14"/>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D183" s="14"/>
-      <c r="E183" s="15"/>
-      <c r="F183" s="15"/>
-      <c r="G183" s="15"/>
-      <c r="H183" s="14"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D184" s="14"/>
-      <c r="E184" s="15"/>
-      <c r="F184" s="15"/>
-      <c r="G184" s="15"/>
-      <c r="H184" s="14"/>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D185" s="14"/>
-      <c r="E185" s="15"/>
-      <c r="F185" s="15"/>
-      <c r="G185" s="15"/>
-      <c r="H185" s="14"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D186" s="14"/>
-      <c r="E186" s="15"/>
-      <c r="F186" s="15"/>
-      <c r="G186" s="15"/>
-      <c r="H186" s="14"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="H119:H130 H134:H138 H142:H143 H1:H61">
+  <conditionalFormatting sqref="H110:H121 H125:H129 H133:H134 H1:H61">
     <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4215,7 +4007,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62:H70">
+  <conditionalFormatting sqref="H62:H67">
     <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4223,7 +4015,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H71:H79">
+  <conditionalFormatting sqref="H68:H73">
     <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4231,7 +4023,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H80:H88">
+  <conditionalFormatting sqref="H74:H79">
     <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4239,7 +4031,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H89:H94">
+  <conditionalFormatting sqref="H80:H85">
     <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4247,7 +4039,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H95:H100">
+  <conditionalFormatting sqref="H86:H91">
     <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4255,7 +4047,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H101:H106">
+  <conditionalFormatting sqref="H92:H97">
     <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4263,7 +4055,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H107:H112">
+  <conditionalFormatting sqref="H98:H103">
     <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4271,7 +4063,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H113:H118">
+  <conditionalFormatting sqref="H104:H109">
     <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4279,7 +4071,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H150:H155">
+  <conditionalFormatting sqref="H141:H146">
     <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4287,7 +4079,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H144:H149">
+  <conditionalFormatting sqref="H135:H140">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4295,7 +4087,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H131:H133">
+  <conditionalFormatting sqref="H122:H124">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4303,7 +4095,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H139:H141">
+  <conditionalFormatting sqref="H130:H132">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update for version 0.7
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{55225790-E440-4FF5-A4B0-DE1DBAFF81DC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA6E3CC8-7B69-421B-BFF8-8020BFC0AFED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{AFF0B8A1-9626-46B3-9A62-F42AFA134D79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="163">
   <si>
     <t>Test Case</t>
   </si>
@@ -219,12 +219,6 @@
     <t>The user should be able to easily enter a new customer with general information</t>
   </si>
   <si>
-    <t>The user should be able to easily enter customer address information for Billing, Shipping, or Other</t>
-  </si>
-  <si>
-    <t>The user should be able to easily enter customer contact information for Primary, Secondary or Other</t>
-  </si>
-  <si>
     <t>Edit</t>
   </si>
   <si>
@@ -325,6 +319,201 @@
   </si>
   <si>
     <t>Record should be displayed because the customer list grid will pull customers that do not yet have contacts associated with them.</t>
+  </si>
+  <si>
+    <t>Select / Click on Customer Name</t>
+  </si>
+  <si>
+    <t>Customer Popup should Load with data.</t>
+  </si>
+  <si>
+    <t>Ensure that the Info Tab is selected</t>
+  </si>
+  <si>
+    <t>Customer Information is displayed</t>
+  </si>
+  <si>
+    <t>Edit Customer Details (Billing Address is Shipping Address, etc.)</t>
+  </si>
+  <si>
+    <t>Values should change when edited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on Save button </t>
+  </si>
+  <si>
+    <t>Message should be displayed that Customer Info was saved</t>
+  </si>
+  <si>
+    <t>Reload Customer by using Step 1, 2, 3</t>
+  </si>
+  <si>
+    <t>Values should show updated values from step 4</t>
+  </si>
+  <si>
+    <t>Message should be displayed that Customer Address Information was saved</t>
+  </si>
+  <si>
+    <t>Message should be displayed that Customer Contact Information was saved</t>
+  </si>
+  <si>
+    <t>Edit Customer Contact Information (Add new, or edit existing)</t>
+  </si>
+  <si>
+    <t>Edit Customer Address Information (Add new,  or edit existing)</t>
+  </si>
+  <si>
+    <t>Remove Customer Address by clicking on Trashcan icon behind the address record</t>
+  </si>
+  <si>
+    <t>Record should be removed from the display</t>
+  </si>
+  <si>
+    <t>Message should be displayed that Customer Information was saved</t>
+  </si>
+  <si>
+    <t>Values should no longer show deleted address value for customer</t>
+  </si>
+  <si>
+    <t>Remove Customer Contact by clicking on Trashcan icon behind the address record</t>
+  </si>
+  <si>
+    <t>Values should no longer show deleted contact value for customer</t>
+  </si>
+  <si>
+    <t>Order Information Grid is displayed</t>
+  </si>
+  <si>
+    <t>Select the Order Tab is selected</t>
+  </si>
+  <si>
+    <t>Verify Orders are for Selected Customer</t>
+  </si>
+  <si>
+    <t>Only orders of the selected Customer is displayed</t>
+  </si>
+  <si>
+    <t>Click on Order Number in List</t>
+  </si>
+  <si>
+    <t>Verify Order Information</t>
+  </si>
+  <si>
+    <t>Order information should be displayed in each tab.</t>
+  </si>
+  <si>
+    <t>Order Detail Display</t>
+  </si>
+  <si>
+    <t>Order Detail popup is displayed with Tabs for Order Info, Tasks, Details, Art, History/Comments, and Correspondence.</t>
+  </si>
+  <si>
+    <t>Verify Order Contact Information changes when contact is selected</t>
+  </si>
+  <si>
+    <t>Prerequisites</t>
+  </si>
+  <si>
+    <t>Order Details screen should be displayed (via Test Case 19)</t>
+  </si>
+  <si>
+    <t>Order Details screen should be displayed (via Test Case 19) - Customer needs to have multiple contacts</t>
+  </si>
+  <si>
+    <t>Select the Contact Dropdown on the Info tab</t>
+  </si>
+  <si>
+    <t>Contact list should be displayed</t>
+  </si>
+  <si>
+    <t>Select a different contact from the dropdown list</t>
+  </si>
+  <si>
+    <t>Contact should be selected and email, phone 1, ext, phone 1 type, phone 2, ext, phone 2 type should update to the values from the selected contact</t>
+  </si>
+  <si>
+    <t>Verify Order History Status Updates</t>
+  </si>
+  <si>
+    <t>Select the Status Dropdown</t>
+  </si>
+  <si>
+    <t>List of statuses should be displayed</t>
+  </si>
+  <si>
+    <t>Select a different status</t>
+  </si>
+  <si>
+    <t>Selected Status should be displayed</t>
+  </si>
+  <si>
+    <t>Save Order and Re-open order</t>
+  </si>
+  <si>
+    <t>Order should come up</t>
+  </si>
+  <si>
+    <t>Verify updated History under History/Comments tab</t>
+  </si>
+  <si>
+    <t>Last updated status should be shown with the user name and current date of logged in user who changed the status.</t>
+  </si>
+  <si>
+    <t>Select the Details Tab</t>
+  </si>
+  <si>
+    <t>Order Details should be displayed with Items, Art Placement, Setup Charges, and Payments displayed</t>
+  </si>
+  <si>
+    <t>Click on the Add button beside the Items title</t>
+  </si>
+  <si>
+    <t>New blank line item should be displayed on the top of the list.</t>
+  </si>
+  <si>
+    <t>Add Order Line Items</t>
+  </si>
+  <si>
+    <t>Items should be updated.  When quantities and price each is entered, there should be an updated SubTotal value.</t>
+  </si>
+  <si>
+    <t>Fill out order details (Item type, color, Y/A, Quantities, Price Each, Vendor, Manufacturer)</t>
+  </si>
+  <si>
+    <t>Select Details Tab</t>
+  </si>
+  <si>
+    <t>Details should display</t>
+  </si>
+  <si>
+    <t>Verify data for newly added Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values should have been saved and loaded. </t>
+  </si>
+  <si>
+    <t>Edit Order Line Items</t>
+  </si>
+  <si>
+    <t>Edit order details (Item type, color, Y/A, Quantities, Price Each, Vendor, Manufacturer)</t>
+  </si>
+  <si>
+    <t>Verify data for Edited Item</t>
+  </si>
+  <si>
+    <t>Delete Order Line Items</t>
+  </si>
+  <si>
+    <t>Iem should be removed from the list</t>
+  </si>
+  <si>
+    <t>Verify data</t>
+  </si>
+  <si>
+    <t>Deleted Line Item should no longer be displayed</t>
+  </si>
+  <si>
+    <t>Delete Order Line Item (Red Trashcan)</t>
   </si>
 </sst>
 </file>
@@ -523,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -583,11 +772,55 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -893,8 +1126,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{606A9948-A2D7-477B-A2E6-4872C5D7E451}">
-      <tableStyleElement type="wholeTable" dxfId="29"/>
-      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="wholeTable" dxfId="33"/>
+      <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1208,10 +1441,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H177"/>
+  <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E181" sqref="E181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2008,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>57</v>
@@ -2204,10 +2437,10 @@
         <v>2</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F56" s="29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G56" s="29"/>
       <c r="H56" s="16"/>
@@ -2220,10 +2453,10 @@
         <v>3</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F57" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G57" s="29"/>
       <c r="H57" s="16"/>
@@ -2236,10 +2469,10 @@
         <v>4</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F58" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G58" s="29"/>
       <c r="H58" s="16"/>
@@ -2252,10 +2485,10 @@
         <v>6</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F59" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G59" s="29"/>
       <c r="H59" s="16"/>
@@ -2268,10 +2501,10 @@
         <v>7</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G60" s="29"/>
       <c r="H60" s="16"/>
@@ -2284,10 +2517,10 @@
         <v>8</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F61" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G61" s="29"/>
       <c r="H61" s="16"/>
@@ -2312,7 +2545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>10</v>
       </c>
@@ -2320,11 +2553,11 @@
         <v>7</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="D63" s="27"/>
       <c r="E63" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F63" s="28"/>
       <c r="G63" s="28"/>
@@ -2350,27 +2583,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="13">
         <v>1</v>
       </c>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="E65" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="G65" s="29"/>
       <c r="H65" s="16"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="13">
         <v>2</v>
       </c>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
+      <c r="E66" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="G66" s="29"/>
       <c r="H66" s="16"/>
     </row>
@@ -2381,196 +2622,214 @@
       <c r="D67" s="13">
         <v>3</v>
       </c>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
+      <c r="E67" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="G67" s="29"/>
       <c r="H67" s="16"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="13">
+        <v>4</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G68" s="29"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="13">
+        <v>5</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69" s="29"/>
+      <c r="H69" s="16"/>
+    </row>
+    <row r="70" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="4">
+        <v>6</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G70" s="29"/>
+      <c r="H70" s="16"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B71" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="30" t="s">
+      <c r="C71" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="30"/>
-      <c r="E68" s="31" t="s">
+      <c r="D71" s="30"/>
+      <c r="E71" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A69" s="6">
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
         <v>11</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" s="27"/>
-      <c r="E69" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="16"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="10" t="s">
+      <c r="C72" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D72" s="27"/>
+      <c r="E72" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="16"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E70" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F70" s="11" t="s">
+      <c r="E73" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H70" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="13">
+      <c r="H73" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="13">
         <v>1</v>
       </c>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="16"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="13">
+      <c r="E74" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F74" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G74" s="29"/>
+      <c r="H74" s="16"/>
+    </row>
+    <row r="75" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="13">
         <v>2</v>
       </c>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="16"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="13">
-        <v>3</v>
-      </c>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
-      <c r="G73" s="29"/>
-      <c r="H73" s="16"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" s="30"/>
-      <c r="E74" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="6">
-        <v>12</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D75" s="27"/>
-      <c r="E75" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
+      <c r="E75" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F75" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="G75" s="29"/>
       <c r="H75" s="16"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="22"/>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H76" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="13">
+        <v>3</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F76" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G76" s="29"/>
+      <c r="H76" s="16"/>
+    </row>
+    <row r="77" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
       <c r="D77" s="13">
-        <v>1</v>
-      </c>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
+        <v>4</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F77" s="29" t="s">
+        <v>103</v>
+      </c>
       <c r="G77" s="29"/>
       <c r="H77" s="16"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
       <c r="D78" s="13">
-        <v>2</v>
-      </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
+        <v>5</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F78" s="29" t="s">
+        <v>108</v>
+      </c>
       <c r="G78" s="29"/>
       <c r="H78" s="16"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
-      <c r="D79" s="13">
-        <v>3</v>
-      </c>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
+      <c r="D79" s="4">
+        <v>6</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>107</v>
+      </c>
       <c r="G79" s="29"/>
       <c r="H79" s="16"/>
     </row>
@@ -2596,17 +2855,17 @@
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D81" s="27"/>
       <c r="E81" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F81" s="28"/>
       <c r="G81" s="28"/>
@@ -2632,27 +2891,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
       <c r="D83" s="13">
         <v>1</v>
       </c>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
+      <c r="E83" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F83" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="G83" s="29"/>
       <c r="H83" s="16"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
       <c r="D84" s="13">
         <v>2</v>
       </c>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
+      <c r="E84" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F84" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="G84" s="29"/>
       <c r="H84" s="16"/>
     </row>
@@ -2663,196 +2930,214 @@
       <c r="D85" s="13">
         <v>3</v>
       </c>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
+      <c r="E85" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F85" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="G85" s="29"/>
       <c r="H85" s="16"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="30" t="s">
+    <row r="86" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="13">
+        <v>4</v>
+      </c>
+      <c r="E86" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F86" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G86" s="29"/>
+      <c r="H86" s="16"/>
+    </row>
+    <row r="87" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="13">
+        <v>5</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F87" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="G87" s="29"/>
+      <c r="H87" s="16"/>
+    </row>
+    <row r="88" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14">
+        <v>6</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G88" s="29"/>
+      <c r="H88" s="16"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="30" t="s">
+      <c r="B89" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C86" s="30" t="s">
+      <c r="C89" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D86" s="30"/>
-      <c r="E86" s="31" t="s">
+      <c r="D89" s="30"/>
+      <c r="E89" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F86" s="31"/>
-      <c r="G86" s="31"/>
-      <c r="H86" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A87" s="6">
-        <v>14</v>
-      </c>
-      <c r="B87" s="6" t="s">
+      <c r="F89" s="31"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>13</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D87" s="27"/>
-      <c r="E87" s="7" t="s">
+      <c r="C90" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D90" s="27"/>
+      <c r="E90" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F87" s="28"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="16"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="22"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="10" t="s">
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="16"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="22"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E88" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F88" s="11" t="s">
+      <c r="E91" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G88" s="11" t="s">
+      <c r="G91" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H88" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="14"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="13">
+      <c r="H91" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="13">
         <v>1</v>
       </c>
-      <c r="E89" s="29"/>
-      <c r="F89" s="29"/>
-      <c r="G89" s="29"/>
-      <c r="H89" s="16"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="14"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="13">
+      <c r="E92" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F92" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G92" s="29"/>
+      <c r="H92" s="16"/>
+    </row>
+    <row r="93" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="13">
         <v>2</v>
       </c>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="16"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="13">
-        <v>3</v>
-      </c>
-      <c r="E91" s="29"/>
-      <c r="F91" s="29"/>
-      <c r="G91" s="29"/>
-      <c r="H91" s="16"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D92" s="30"/>
-      <c r="E92" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" s="31"/>
-      <c r="G92" s="31"/>
-      <c r="H92" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="6">
-        <v>15</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D93" s="27"/>
-      <c r="E93" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F93" s="28"/>
-      <c r="G93" s="28"/>
+      <c r="E93" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F93" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="G93" s="29"/>
       <c r="H93" s="16"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="22"/>
-      <c r="B94" s="22"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F94" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G94" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H94" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="13">
+        <v>3</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F94" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G94" s="29"/>
+      <c r="H94" s="16"/>
+    </row>
+    <row r="95" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
       <c r="D95" s="13">
-        <v>1</v>
-      </c>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
+        <v>4</v>
+      </c>
+      <c r="E95" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="G95" s="29"/>
       <c r="H95" s="16"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
       <c r="D96" s="13">
-        <v>2</v>
-      </c>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
+        <v>5</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F96" s="29" t="s">
+        <v>114</v>
+      </c>
       <c r="G96" s="29"/>
       <c r="H96" s="16"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="14"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
-      <c r="D97" s="13">
-        <v>3</v>
-      </c>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
+      <c r="D97" s="14">
+        <v>6</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>115</v>
+      </c>
       <c r="G97" s="29"/>
       <c r="H97" s="16"/>
     </row>
@@ -2878,17 +3163,17 @@
     </row>
     <row r="99" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D99" s="27"/>
       <c r="E99" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F99" s="28"/>
       <c r="G99" s="28"/>
@@ -2914,27 +3199,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A101" s="14"/>
       <c r="B101" s="14"/>
       <c r="C101" s="14"/>
       <c r="D101" s="13">
         <v>1</v>
       </c>
-      <c r="E101" s="29"/>
-      <c r="F101" s="29"/>
+      <c r="E101" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F101" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="G101" s="29"/>
       <c r="H101" s="16"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="14"/>
       <c r="B102" s="14"/>
       <c r="C102" s="14"/>
       <c r="D102" s="13">
         <v>2</v>
       </c>
-      <c r="E102" s="29"/>
-      <c r="F102" s="29"/>
+      <c r="E102" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F102" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="G102" s="29"/>
       <c r="H102" s="16"/>
     </row>
@@ -2945,930 +3238,1080 @@
       <c r="D103" s="13">
         <v>3</v>
       </c>
-      <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
+      <c r="E103" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F103" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="G103" s="29"/>
       <c r="H103" s="16"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="30" t="s">
+    <row r="104" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="13">
+        <v>4</v>
+      </c>
+      <c r="E104" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F104" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G104" s="29"/>
+      <c r="H104" s="16"/>
+    </row>
+    <row r="105" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="13">
+        <v>5</v>
+      </c>
+      <c r="E105" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F105" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="G105" s="29"/>
+      <c r="H105" s="16"/>
+    </row>
+    <row r="106" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14">
+        <v>6</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F106" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G106" s="29"/>
+      <c r="H106" s="16"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B104" s="30" t="s">
+      <c r="B107" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C104" s="30" t="s">
+      <c r="C107" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D104" s="30"/>
-      <c r="E104" s="31" t="s">
+      <c r="D107" s="30"/>
+      <c r="E107" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F104" s="31"/>
-      <c r="G104" s="31"/>
-      <c r="H104" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A105" s="6">
-        <v>17</v>
-      </c>
-      <c r="B105" s="6" t="s">
+      <c r="F107" s="31"/>
+      <c r="G107" s="31"/>
+      <c r="H107" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A108" s="6">
+        <v>15</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D105" s="27"/>
-      <c r="E105" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F105" s="28"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="16"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="22"/>
-      <c r="B106" s="22"/>
-      <c r="C106" s="22"/>
-      <c r="D106" s="10" t="s">
+      <c r="C108" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D108" s="27"/>
+      <c r="E108" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F108" s="28"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="16"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="22"/>
+      <c r="B109" s="22"/>
+      <c r="C109" s="22"/>
+      <c r="D109" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E106" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F106" s="11" t="s">
+      <c r="E109" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F109" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G106" s="11" t="s">
+      <c r="G109" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H106" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
-      <c r="D107" s="13">
+      <c r="H109" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A110" s="14"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="13">
         <v>1</v>
       </c>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="16"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="14"/>
-      <c r="D108" s="13">
+      <c r="E110" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F110" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G110" s="29"/>
+      <c r="H110" s="16"/>
+    </row>
+    <row r="111" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="13">
         <v>2</v>
       </c>
-      <c r="E108" s="29"/>
-      <c r="F108" s="29"/>
-      <c r="G108" s="29"/>
-      <c r="H108" s="16"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="13">
-        <v>3</v>
-      </c>
-      <c r="E109" s="29"/>
-      <c r="F109" s="29"/>
-      <c r="G109" s="29"/>
-      <c r="H109" s="16"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D110" s="25"/>
-      <c r="E110" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F110" s="26"/>
-      <c r="G110" s="26"/>
-      <c r="H110" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A111" s="6">
-        <v>18</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D111" s="27"/>
-      <c r="E111" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F111" s="28"/>
-      <c r="G111" s="28"/>
+      <c r="E111" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F111" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="G111" s="29"/>
       <c r="H111" s="16"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="22"/>
-      <c r="B112" s="22"/>
-      <c r="C112" s="22"/>
-      <c r="D112" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E112" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F112" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G112" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H112" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="13">
+        <v>3</v>
+      </c>
+      <c r="E112" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F112" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="G112" s="29"/>
+      <c r="H112" s="16"/>
+    </row>
+    <row r="113" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A113" s="14"/>
       <c r="B113" s="14"/>
       <c r="C113" s="14"/>
-      <c r="D113" s="13">
+      <c r="D113" s="14">
+        <v>4</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F113" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G113" s="29"/>
+      <c r="H113" s="16"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E113" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F113" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G113" s="23"/>
-      <c r="H113" s="16"/>
-    </row>
-    <row r="114" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="13">
+      <c r="C114" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" s="25"/>
+      <c r="E114" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F114" s="26"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A115" s="6">
+        <v>16</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D115" s="27"/>
+      <c r="E115" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F115" s="28"/>
+      <c r="G115" s="28"/>
+      <c r="H115" s="16"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="22"/>
+      <c r="B116" s="22"/>
+      <c r="C116" s="22"/>
+      <c r="D116" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E114" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F114" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G114" s="23"/>
-      <c r="H114" s="16"/>
-    </row>
-    <row r="115" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A115" s="14"/>
-      <c r="B115" s="14"/>
-      <c r="C115" s="14"/>
-      <c r="D115" s="13">
-        <v>3</v>
-      </c>
-      <c r="E115" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F115" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G115" s="23"/>
-      <c r="H115" s="16"/>
-    </row>
-    <row r="116" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A116" s="14"/>
-      <c r="B116" s="14"/>
-      <c r="C116" s="14"/>
-      <c r="D116" s="13">
-        <v>3</v>
-      </c>
-      <c r="E116" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="F116" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="G116" s="23"/>
-      <c r="H116" s="16"/>
-    </row>
-    <row r="117" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="E116" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F116" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H116" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A117" s="14"/>
       <c r="B117" s="14"/>
       <c r="C117" s="14"/>
       <c r="D117" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E117" s="29" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="F117" s="29" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G117" s="23"/>
       <c r="H117" s="16"/>
     </row>
-    <row r="118" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="14"/>
       <c r="B118" s="14"/>
       <c r="C118" s="14"/>
       <c r="D118" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F118" s="29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G118" s="23"/>
       <c r="H118" s="16"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B119" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D119" s="30"/>
-      <c r="E119" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F119" s="31"/>
-      <c r="G119" s="31"/>
-      <c r="H119" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A120" s="6">
-        <v>19</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D120" s="27"/>
-      <c r="E120" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F120" s="28"/>
-      <c r="G120" s="28"/>
+    <row r="119" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A119" s="14"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="14"/>
+      <c r="D119" s="13">
+        <v>3</v>
+      </c>
+      <c r="E119" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F119" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G119" s="23"/>
+      <c r="H119" s="16"/>
+    </row>
+    <row r="120" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="13">
+        <v>3</v>
+      </c>
+      <c r="E120" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F120" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G120" s="23"/>
       <c r="H120" s="16"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="22"/>
-      <c r="B121" s="22"/>
-      <c r="C121" s="22"/>
-      <c r="D121" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E121" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F121" s="11" t="s">
+    <row r="121" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="14"/>
+      <c r="D121" s="13">
         <v>4</v>
       </c>
-      <c r="G121" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H121" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="E121" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F121" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G121" s="23"/>
+      <c r="H121" s="16"/>
+    </row>
+    <row r="122" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="14"/>
       <c r="B122" s="14"/>
       <c r="C122" s="14"/>
       <c r="D122" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E122" s="29" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="F122" s="29" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="G122" s="23"/>
       <c r="H122" s="16"/>
     </row>
-    <row r="123" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A123" s="14"/>
-      <c r="B123" s="14"/>
-      <c r="C123" s="14"/>
-      <c r="D123" s="13">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="30"/>
+      <c r="E123" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F123" s="31"/>
+      <c r="G123" s="31"/>
+      <c r="H123" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A124" s="6">
+        <v>17</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D124" s="27"/>
+      <c r="E124" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F124" s="28"/>
+      <c r="G124" s="28"/>
+      <c r="H124" s="16"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="22"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="22"/>
+      <c r="D125" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E123" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F123" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G123" s="23"/>
-      <c r="H123" s="16"/>
-    </row>
-    <row r="124" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14"/>
-      <c r="C124" s="14"/>
-      <c r="D124" s="13">
-        <v>3</v>
-      </c>
-      <c r="E124" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F124" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G124" s="23"/>
-      <c r="H124" s="16"/>
-    </row>
-    <row r="125" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A125" s="14"/>
-      <c r="B125" s="14"/>
-      <c r="C125" s="14"/>
-      <c r="D125" s="13">
+      <c r="E125" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F125" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E125" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F125" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G125" s="29"/>
-      <c r="H125" s="16"/>
-    </row>
-    <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G125" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H125" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A126" s="14"/>
       <c r="B126" s="14"/>
       <c r="C126" s="14"/>
       <c r="D126" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E126" s="29" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F126" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="G126" s="29"/>
+        <v>32</v>
+      </c>
+      <c r="G126" s="23"/>
       <c r="H126" s="16"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B127" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D127" s="30"/>
-      <c r="E127" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F127" s="31"/>
-      <c r="G127" s="31"/>
-      <c r="H127" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A128" s="6">
-        <v>20</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C128" s="6" t="s">
+    <row r="127" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A127" s="14"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="13">
+        <v>2</v>
+      </c>
+      <c r="E127" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D128" s="27"/>
-      <c r="E128" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F128" s="28"/>
-      <c r="G128" s="28"/>
+      <c r="F127" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G127" s="23"/>
+      <c r="H127" s="16"/>
+    </row>
+    <row r="128" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A128" s="14"/>
+      <c r="B128" s="14"/>
+      <c r="C128" s="14"/>
+      <c r="D128" s="13">
+        <v>3</v>
+      </c>
+      <c r="E128" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F128" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G128" s="23"/>
       <c r="H128" s="16"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="22"/>
-      <c r="B129" s="22"/>
-      <c r="C129" s="22"/>
-      <c r="D129" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E129" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F129" s="11" t="s">
+    <row r="129" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A129" s="14"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="14"/>
+      <c r="D129" s="13">
         <v>4</v>
       </c>
-      <c r="G129" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H129" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="E129" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F129" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="G129" s="29"/>
+      <c r="H129" s="16"/>
+    </row>
+    <row r="130" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A130" s="14"/>
       <c r="B130" s="14"/>
       <c r="C130" s="14"/>
       <c r="D130" s="13">
+        <v>5</v>
+      </c>
+      <c r="E130" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F130" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G130" s="29"/>
+      <c r="H130" s="16"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E130" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F130" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G130" s="23"/>
-      <c r="H130" s="16"/>
-    </row>
-    <row r="131" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A131" s="14"/>
-      <c r="B131" s="14"/>
-      <c r="C131" s="14"/>
-      <c r="D131" s="13">
+      <c r="C131" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D131" s="30"/>
+      <c r="E131" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F131" s="31"/>
+      <c r="G131" s="31"/>
+      <c r="H131" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A132" s="6">
+        <v>18</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D132" s="27"/>
+      <c r="E132" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F132" s="28"/>
+      <c r="G132" s="28"/>
+      <c r="H132" s="16"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="22"/>
+      <c r="B133" s="22"/>
+      <c r="C133" s="22"/>
+      <c r="D133" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E131" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F131" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G131" s="23"/>
-      <c r="H131" s="16"/>
-    </row>
-    <row r="132" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A132" s="14"/>
-      <c r="B132" s="14"/>
-      <c r="C132" s="14"/>
-      <c r="D132" s="13">
-        <v>3</v>
-      </c>
-      <c r="E132" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F132" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G132" s="23"/>
-      <c r="H132" s="16"/>
-    </row>
-    <row r="133" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A133" s="14"/>
-      <c r="B133" s="14"/>
-      <c r="C133" s="14"/>
-      <c r="D133" s="13">
-        <v>2</v>
-      </c>
-      <c r="E133" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F133" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="G133" s="29"/>
-      <c r="H133" s="16"/>
-    </row>
-    <row r="134" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E133" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F133" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G133" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H133" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A134" s="14"/>
       <c r="B134" s="14"/>
       <c r="C134" s="14"/>
       <c r="D134" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="F134" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="G134" s="29"/>
+        <v>32</v>
+      </c>
+      <c r="G134" s="23"/>
       <c r="H134" s="16"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B135" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C135" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D135" s="30"/>
-      <c r="E135" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F135" s="31"/>
-      <c r="G135" s="31"/>
-      <c r="H135" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A136" s="6">
-        <v>21</v>
-      </c>
-      <c r="B136" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136" s="6" t="s">
+    <row r="135" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A135" s="14"/>
+      <c r="B135" s="14"/>
+      <c r="C135" s="14"/>
+      <c r="D135" s="13">
+        <v>2</v>
+      </c>
+      <c r="E135" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D136" s="27"/>
-      <c r="E136" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F136" s="28"/>
-      <c r="G136" s="28"/>
+      <c r="F135" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G135" s="23"/>
+      <c r="H135" s="16"/>
+    </row>
+    <row r="136" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A136" s="14"/>
+      <c r="B136" s="14"/>
+      <c r="C136" s="14"/>
+      <c r="D136" s="13">
+        <v>3</v>
+      </c>
+      <c r="E136" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F136" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G136" s="23"/>
       <c r="H136" s="16"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="22"/>
-      <c r="B137" s="22"/>
-      <c r="C137" s="22"/>
-      <c r="D137" s="10" t="s">
+    <row r="137" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A137" s="14"/>
+      <c r="B137" s="14"/>
+      <c r="C137" s="14"/>
+      <c r="D137" s="13">
         <v>2</v>
       </c>
-      <c r="E137" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F137" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G137" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H137" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E137" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F137" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G137" s="29"/>
+      <c r="H137" s="16"/>
+    </row>
+    <row r="138" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A138" s="14"/>
       <c r="B138" s="14"/>
       <c r="C138" s="14"/>
       <c r="D138" s="13">
-        <v>1</v>
-      </c>
-      <c r="E138" s="29"/>
-      <c r="F138" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="E138" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F138" s="29" t="s">
+        <v>57</v>
+      </c>
       <c r="G138" s="29"/>
       <c r="H138" s="16"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="14"/>
-      <c r="B139" s="14"/>
-      <c r="C139" s="14"/>
-      <c r="D139" s="13">
+      <c r="A139" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D139" s="30"/>
+      <c r="E139" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F139" s="31"/>
+      <c r="G139" s="31"/>
+      <c r="H139" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A140" s="6">
+        <v>19</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D140" s="27"/>
+      <c r="E140" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F140" s="28"/>
+      <c r="G140" s="28"/>
+      <c r="H140" s="16"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="22"/>
+      <c r="B141" s="22"/>
+      <c r="C141" s="22"/>
+      <c r="D141" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E139" s="29"/>
-      <c r="F139" s="29"/>
-      <c r="G139" s="29"/>
-      <c r="H139" s="16"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="14"/>
-      <c r="B140" s="14"/>
-      <c r="C140" s="14"/>
-      <c r="D140" s="13">
-        <v>3</v>
-      </c>
-      <c r="E140" s="29"/>
-      <c r="F140" s="29"/>
-      <c r="G140" s="29"/>
-      <c r="H140" s="16"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B141" s="30" t="s">
+      <c r="E141" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F141" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G141" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H141" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="14"/>
+      <c r="D142" s="13">
         <v>1</v>
       </c>
-      <c r="C141" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D141" s="30"/>
-      <c r="E141" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F141" s="31"/>
-      <c r="G141" s="31"/>
-      <c r="H141" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A142" s="6">
-        <v>22</v>
-      </c>
-      <c r="B142" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D142" s="27"/>
-      <c r="E142" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F142" s="28"/>
-      <c r="G142" s="28"/>
+      <c r="E142" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F142" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G142" s="23"/>
       <c r="H142" s="16"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A143" s="22"/>
-      <c r="B143" s="22"/>
-      <c r="C143" s="22"/>
-      <c r="D143" s="10" t="s">
+    <row r="143" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A143" s="14"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="14"/>
+      <c r="D143" s="13">
         <v>2</v>
       </c>
-      <c r="E143" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F143" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G143" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H143" s="34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E143" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F143" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G143" s="23"/>
+      <c r="H143" s="16"/>
+    </row>
+    <row r="144" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A144" s="14"/>
       <c r="B144" s="14"/>
       <c r="C144" s="14"/>
       <c r="D144" s="13">
-        <v>1</v>
-      </c>
-      <c r="E144" s="29"/>
-      <c r="F144" s="29"/>
-      <c r="G144" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="E144" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F144" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G144" s="23"/>
       <c r="H144" s="16"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A145" s="14"/>
       <c r="B145" s="14"/>
       <c r="C145" s="14"/>
       <c r="D145" s="13">
-        <v>2</v>
-      </c>
-      <c r="E145" s="29"/>
-      <c r="F145" s="29"/>
+        <v>4</v>
+      </c>
+      <c r="E145" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F145" s="29" t="s">
+        <v>126</v>
+      </c>
       <c r="G145" s="29"/>
       <c r="H145" s="16"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A146" s="14"/>
       <c r="B146" s="14"/>
       <c r="C146" s="14"/>
       <c r="D146" s="13">
-        <v>3</v>
-      </c>
-      <c r="E146" s="29"/>
-      <c r="F146" s="29"/>
+        <v>5</v>
+      </c>
+      <c r="E146" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F146" s="29" t="s">
+        <v>124</v>
+      </c>
       <c r="G146" s="29"/>
       <c r="H146" s="16"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A147" s="14"/>
-      <c r="B147" s="14"/>
-      <c r="C147" s="14"/>
-      <c r="D147" s="13"/>
-      <c r="E147" s="29"/>
-      <c r="F147" s="29"/>
-      <c r="G147" s="29"/>
-      <c r="H147" s="13"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A148" s="14"/>
-      <c r="B148" s="14"/>
-      <c r="C148" s="14"/>
-      <c r="D148" s="13"/>
-      <c r="E148" s="29"/>
-      <c r="F148" s="29"/>
-      <c r="G148" s="29"/>
-      <c r="H148" s="13"/>
+      <c r="A147" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D147" s="30"/>
+      <c r="E147" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F147" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G147" s="31"/>
+      <c r="H147" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A148" s="6">
+        <v>20</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D148" s="27"/>
+      <c r="E148" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F148" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G148" s="28"/>
+      <c r="H148" s="16"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A149" s="14"/>
-      <c r="B149" s="14"/>
-      <c r="C149" s="14"/>
-      <c r="D149" s="13"/>
-      <c r="E149" s="29"/>
-      <c r="F149" s="29"/>
-      <c r="G149" s="29"/>
-      <c r="H149" s="13"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="22"/>
+      <c r="B149" s="22"/>
+      <c r="C149" s="22"/>
+      <c r="D149" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E149" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F149" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G149" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H149" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A150" s="14"/>
       <c r="B150" s="14"/>
       <c r="C150" s="14"/>
-      <c r="D150" s="14"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="15"/>
-      <c r="G150" s="15"/>
-      <c r="H150" s="14"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A151" s="14">
+      <c r="D150" s="13">
+        <v>1</v>
+      </c>
+      <c r="E150" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="F150" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="G150" s="29"/>
+      <c r="H150" s="16"/>
+    </row>
+    <row r="151" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A151" s="14"/>
+      <c r="B151" s="14"/>
+      <c r="C151" s="14"/>
+      <c r="D151" s="13">
+        <v>2</v>
+      </c>
+      <c r="E151" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="F151" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G151" s="29"/>
+      <c r="H151" s="16"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D152" s="30"/>
+      <c r="E152" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F152" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G152" s="31"/>
+      <c r="H152" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A153" s="6">
+        <v>21</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D153" s="27"/>
+      <c r="E153" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F153" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G153" s="28"/>
+      <c r="H153" s="16"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="22"/>
+      <c r="B154" s="22"/>
+      <c r="C154" s="22"/>
+      <c r="D154" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E154" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F154" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G154" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B151" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C151" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D151" s="14"/>
-      <c r="E151" s="15"/>
-      <c r="F151" s="15"/>
-      <c r="G151" s="15"/>
-      <c r="H151" s="14"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A152" s="14"/>
-      <c r="B152" s="14"/>
-      <c r="C152" s="14"/>
-      <c r="D152" s="14"/>
-      <c r="E152" s="15"/>
-      <c r="F152" s="15"/>
-      <c r="G152" s="15"/>
-      <c r="H152" s="14"/>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A153" s="14">
-        <v>7</v>
-      </c>
-      <c r="B153" s="14"/>
-      <c r="C153" s="14"/>
-      <c r="D153" s="14"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
-      <c r="G153" s="15"/>
-      <c r="H153" s="14"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A154" s="14">
-        <v>8</v>
-      </c>
-      <c r="B154" s="14"/>
-      <c r="C154" s="14"/>
-      <c r="D154" s="14"/>
-      <c r="E154" s="15"/>
-      <c r="F154" s="15"/>
-      <c r="G154" s="15"/>
-      <c r="H154" s="14"/>
+      <c r="H154" s="34" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A155" s="14">
-        <v>9</v>
-      </c>
+      <c r="A155" s="14"/>
       <c r="B155" s="14"/>
       <c r="C155" s="14"/>
-      <c r="D155" s="14"/>
-      <c r="E155" s="15"/>
-      <c r="F155" s="15"/>
-      <c r="G155" s="15"/>
-      <c r="H155" s="14"/>
+      <c r="D155" s="13">
+        <v>1</v>
+      </c>
+      <c r="E155" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="F155" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="G155" s="29"/>
+      <c r="H155" s="16"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A156" s="14">
-        <v>10</v>
-      </c>
+      <c r="A156" s="14"/>
       <c r="B156" s="14"/>
       <c r="C156" s="14"/>
-      <c r="D156" s="14"/>
-      <c r="E156" s="15"/>
-      <c r="F156" s="15"/>
-      <c r="G156" s="15"/>
-      <c r="H156" s="14"/>
+      <c r="D156" s="13">
+        <v>2</v>
+      </c>
+      <c r="E156" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="F156" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="G156" s="29"/>
+      <c r="H156" s="16"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A157" s="14">
-        <v>11</v>
-      </c>
+      <c r="A157" s="14"/>
       <c r="B157" s="14"/>
       <c r="C157" s="14"/>
-      <c r="D157" s="14"/>
-      <c r="E157" s="15"/>
-      <c r="F157" s="15"/>
+      <c r="D157" s="14">
+        <v>3</v>
+      </c>
+      <c r="E157" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F157" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="G157" s="15"/>
       <c r="H157" s="14"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A158" s="14">
-        <v>12</v>
-      </c>
+    <row r="158" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A158" s="14"/>
       <c r="B158" s="14"/>
       <c r="C158" s="14"/>
-      <c r="D158" s="14"/>
-      <c r="E158" s="15"/>
-      <c r="F158" s="15"/>
+      <c r="D158" s="14">
+        <v>4</v>
+      </c>
+      <c r="E158" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F158" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="G158" s="15"/>
       <c r="H158" s="14"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A159" s="14">
-        <v>13</v>
-      </c>
-      <c r="B159" s="14"/>
-      <c r="C159" s="14"/>
-      <c r="D159" s="14"/>
-      <c r="E159" s="15"/>
-      <c r="F159" s="15"/>
-      <c r="G159" s="15"/>
-      <c r="H159" s="14"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A160" s="14">
-        <v>14</v>
-      </c>
-      <c r="B160" s="14"/>
-      <c r="C160" s="14"/>
-      <c r="D160" s="14"/>
-      <c r="E160" s="15"/>
-      <c r="F160" s="15"/>
-      <c r="G160" s="15"/>
-      <c r="H160" s="14"/>
+      <c r="A159" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B159" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C159" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D159" s="30"/>
+      <c r="E159" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F159" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G159" s="31"/>
+      <c r="H159" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A160" s="6">
+        <v>22</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D160" s="27"/>
+      <c r="E160" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F160" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G160" s="28"/>
+      <c r="H160" s="16"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="14">
-        <v>15</v>
-      </c>
-      <c r="B161" s="14"/>
-      <c r="C161" s="14"/>
-      <c r="D161" s="14"/>
-      <c r="E161" s="15"/>
-      <c r="F161" s="15"/>
-      <c r="G161" s="15"/>
-      <c r="H161" s="14"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A162" s="14">
-        <v>16</v>
-      </c>
+      <c r="A161" s="22"/>
+      <c r="B161" s="22"/>
+      <c r="C161" s="22"/>
+      <c r="D161" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E161" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F161" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G161" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H161" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A162" s="14"/>
       <c r="B162" s="14"/>
       <c r="C162" s="14"/>
-      <c r="D162" s="14"/>
-      <c r="E162" s="15"/>
-      <c r="F162" s="15"/>
-      <c r="G162" s="15"/>
-      <c r="H162" s="14"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A163" s="14">
-        <v>17</v>
-      </c>
+      <c r="D162" s="13">
+        <v>1</v>
+      </c>
+      <c r="E162" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="F162" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="G162" s="29"/>
+      <c r="H162" s="16"/>
+    </row>
+    <row r="163" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A163" s="14"/>
       <c r="B163" s="14"/>
       <c r="C163" s="14"/>
-      <c r="D163" s="14"/>
-      <c r="E163" s="15"/>
-      <c r="F163" s="15"/>
-      <c r="G163" s="15"/>
-      <c r="H163" s="14"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A164" s="14">
-        <v>18</v>
-      </c>
+      <c r="D163" s="13">
+        <v>2</v>
+      </c>
+      <c r="E163" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="F163" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="G163" s="29"/>
+      <c r="H163" s="16"/>
+    </row>
+    <row r="164" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A164" s="14"/>
       <c r="B164" s="14"/>
       <c r="C164" s="14"/>
-      <c r="D164" s="14"/>
-      <c r="E164" s="15"/>
-      <c r="F164" s="15"/>
+      <c r="D164" s="14">
+        <v>3</v>
+      </c>
+      <c r="E164" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F164" s="15" t="s">
+        <v>149</v>
+      </c>
       <c r="G164" s="15"/>
       <c r="H164" s="14"/>
     </row>
@@ -3876,9 +4319,15 @@
       <c r="A165" s="14"/>
       <c r="B165" s="14"/>
       <c r="C165" s="14"/>
-      <c r="D165" s="14"/>
-      <c r="E165" s="15"/>
-      <c r="F165" s="15"/>
+      <c r="D165" s="14">
+        <v>4</v>
+      </c>
+      <c r="E165" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F165" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="G165" s="15"/>
       <c r="H165" s="14"/>
     </row>
@@ -3886,69 +4335,125 @@
       <c r="A166" s="14"/>
       <c r="B166" s="14"/>
       <c r="C166" s="14"/>
-      <c r="D166" s="14"/>
-      <c r="E166" s="15"/>
-      <c r="F166" s="15"/>
+      <c r="D166" s="14">
+        <v>5</v>
+      </c>
+      <c r="E166" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F166" s="15" t="s">
+        <v>152</v>
+      </c>
       <c r="G166" s="15"/>
       <c r="H166" s="14"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A167" s="14"/>
       <c r="B167" s="14"/>
       <c r="C167" s="14"/>
-      <c r="D167" s="14"/>
-      <c r="E167" s="15"/>
-      <c r="F167" s="15"/>
+      <c r="D167" s="14">
+        <v>6</v>
+      </c>
+      <c r="E167" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F167" s="15" t="s">
+        <v>154</v>
+      </c>
       <c r="G167" s="15"/>
       <c r="H167" s="14"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A168" s="14"/>
-      <c r="B168" s="14"/>
-      <c r="C168" s="14"/>
-      <c r="D168" s="14"/>
-      <c r="E168" s="15"/>
-      <c r="F168" s="15"/>
-      <c r="G168" s="15"/>
-      <c r="H168" s="14"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A169" s="14"/>
-      <c r="B169" s="14"/>
-      <c r="C169" s="14"/>
-      <c r="D169" s="14"/>
-      <c r="E169" s="15"/>
-      <c r="F169" s="15"/>
-      <c r="G169" s="15"/>
-      <c r="H169" s="14"/>
+      <c r="A168" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B168" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D168" s="30"/>
+      <c r="E168" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F168" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G168" s="31"/>
+      <c r="H168" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A169" s="6">
+        <v>22</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D169" s="27"/>
+      <c r="E169" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G169" s="28"/>
+      <c r="H169" s="16"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A170" s="14"/>
-      <c r="B170" s="14"/>
-      <c r="C170" s="14"/>
-      <c r="D170" s="14"/>
-      <c r="E170" s="15"/>
-      <c r="F170" s="15"/>
-      <c r="G170" s="15"/>
-      <c r="H170" s="14"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" s="22"/>
+      <c r="B170" s="22"/>
+      <c r="C170" s="22"/>
+      <c r="D170" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E170" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F170" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G170" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H170" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A171" s="14"/>
       <c r="B171" s="14"/>
       <c r="C171" s="14"/>
-      <c r="D171" s="14"/>
-      <c r="E171" s="15"/>
-      <c r="F171" s="15"/>
-      <c r="G171" s="15"/>
-      <c r="H171" s="14"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D171" s="13">
+        <v>1</v>
+      </c>
+      <c r="E171" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="F171" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="G171" s="29"/>
+      <c r="H171" s="16"/>
+    </row>
+    <row r="172" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A172" s="14"/>
       <c r="B172" s="14"/>
       <c r="C172" s="14"/>
-      <c r="D172" s="14"/>
-      <c r="E172" s="15"/>
-      <c r="F172" s="15"/>
+      <c r="D172" s="14">
+        <v>3</v>
+      </c>
+      <c r="E172" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F172" s="15" t="s">
+        <v>149</v>
+      </c>
       <c r="G172" s="15"/>
       <c r="H172" s="14"/>
     </row>
@@ -3956,42 +4461,268 @@
       <c r="A173" s="14"/>
       <c r="B173" s="14"/>
       <c r="C173" s="14"/>
-      <c r="D173" s="14"/>
-      <c r="E173" s="15"/>
-      <c r="F173" s="15"/>
+      <c r="D173" s="14">
+        <v>4</v>
+      </c>
+      <c r="E173" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F173" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="G173" s="15"/>
       <c r="H173" s="14"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D174" s="14"/>
-      <c r="E174" s="15"/>
-      <c r="F174" s="15"/>
+      <c r="A174" s="14"/>
+      <c r="B174" s="14"/>
+      <c r="C174" s="14"/>
+      <c r="D174" s="14">
+        <v>5</v>
+      </c>
+      <c r="E174" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F174" s="15" t="s">
+        <v>152</v>
+      </c>
       <c r="G174" s="15"/>
       <c r="H174" s="14"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D175" s="14"/>
-      <c r="E175" s="15"/>
-      <c r="F175" s="15"/>
+    <row r="175" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A175" s="14"/>
+      <c r="B175" s="14"/>
+      <c r="C175" s="14"/>
+      <c r="D175" s="14">
+        <v>6</v>
+      </c>
+      <c r="E175" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F175" s="15" t="s">
+        <v>154</v>
+      </c>
       <c r="G175" s="15"/>
       <c r="H175" s="14"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D176" s="14"/>
-      <c r="E176" s="15"/>
-      <c r="F176" s="15"/>
-      <c r="G176" s="15"/>
-      <c r="H176" s="14"/>
-    </row>
-    <row r="177" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D177" s="14"/>
-      <c r="E177" s="15"/>
-      <c r="F177" s="15"/>
-      <c r="G177" s="15"/>
-      <c r="H177" s="14"/>
+      <c r="A176" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B176" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D176" s="30"/>
+      <c r="E176" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F176" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G176" s="31"/>
+      <c r="H176" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A177" s="6">
+        <v>22</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D177" s="27"/>
+      <c r="E177" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F177" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G177" s="28"/>
+      <c r="H177" s="16"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" s="22"/>
+      <c r="B178" s="22"/>
+      <c r="C178" s="22"/>
+      <c r="D178" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E178" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F178" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G178" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H178" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A179" s="14"/>
+      <c r="B179" s="14"/>
+      <c r="C179" s="14"/>
+      <c r="D179" s="13">
+        <v>1</v>
+      </c>
+      <c r="E179" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="F179" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="G179" s="29"/>
+      <c r="H179" s="16"/>
+    </row>
+    <row r="180" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A180" s="14"/>
+      <c r="B180" s="14"/>
+      <c r="C180" s="14"/>
+      <c r="D180" s="14">
+        <v>3</v>
+      </c>
+      <c r="E180" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F180" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G180" s="15"/>
+      <c r="H180" s="14"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" s="14"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="14"/>
+      <c r="D181" s="14">
+        <v>4</v>
+      </c>
+      <c r="E181" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F181" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G181" s="15"/>
+      <c r="H181" s="14"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" s="14"/>
+      <c r="B182" s="14"/>
+      <c r="C182" s="14"/>
+      <c r="D182" s="14">
+        <v>5</v>
+      </c>
+      <c r="E182" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F182" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G182" s="15"/>
+      <c r="H182" s="14"/>
+    </row>
+    <row r="183" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A183" s="14"/>
+      <c r="B183" s="14"/>
+      <c r="C183" s="14"/>
+      <c r="D183" s="14">
+        <v>6</v>
+      </c>
+      <c r="E183" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F183" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G183" s="15"/>
+      <c r="H183" s="14"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184" s="14"/>
+      <c r="B184" s="14"/>
+      <c r="C184" s="14"/>
+      <c r="D184" s="14"/>
+      <c r="E184" s="15"/>
+      <c r="F184" s="15"/>
+      <c r="G184" s="15"/>
+      <c r="H184" s="14"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185" s="14"/>
+      <c r="B185" s="14"/>
+      <c r="C185" s="14"/>
+      <c r="D185" s="14"/>
+      <c r="E185" s="15"/>
+      <c r="F185" s="15"/>
+      <c r="G185" s="15"/>
+      <c r="H185" s="14"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" s="14"/>
+      <c r="B186" s="14"/>
+      <c r="C186" s="14"/>
+      <c r="D186" s="14"/>
+      <c r="E186" s="15"/>
+      <c r="F186" s="15"/>
+      <c r="G186" s="15"/>
+      <c r="H186" s="14"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D187" s="35"/>
+      <c r="E187" s="36"/>
+      <c r="F187" s="36"/>
+      <c r="G187" s="36"/>
+      <c r="H187" s="35"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D188" s="35"/>
+      <c r="E188" s="36"/>
+      <c r="F188" s="36"/>
+      <c r="G188" s="36"/>
+      <c r="H188" s="35"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D189" s="35"/>
+      <c r="E189" s="36"/>
+      <c r="F189" s="36"/>
+      <c r="G189" s="36"/>
+      <c r="H189" s="35"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D190" s="35"/>
+      <c r="E190" s="36"/>
+      <c r="F190" s="36"/>
+      <c r="G190" s="36"/>
+      <c r="H190" s="35"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H110:H121 H125:H129 H133:H134 H1:H61">
+  <conditionalFormatting sqref="H114:H125 H129:H133 H1:H61 H137:H141 H145:H146">
+    <cfRule type="cellIs" dxfId="31" priority="43" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="44" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" dxfId="29" priority="41" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="42" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62:H70">
     <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3999,7 +4730,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H71:H79">
     <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4007,87 +4738,87 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62:H67">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+  <conditionalFormatting sqref="H80:H88">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68:H73">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+  <conditionalFormatting sqref="H89:H97">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H74:H79">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+  <conditionalFormatting sqref="H98:H106">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H80:H85">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+  <conditionalFormatting sqref="H107:H113">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H86:H91">
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+  <conditionalFormatting sqref="H147:H151">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H92:H97">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+  <conditionalFormatting sqref="H126:H128">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H98:H103">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+  <conditionalFormatting sqref="H134:H136">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H104:H109">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+  <conditionalFormatting sqref="H142:H144">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H141:H146">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+  <conditionalFormatting sqref="H152:H156">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H135:H140">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+  <conditionalFormatting sqref="H159:H163">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H122:H124">
+  <conditionalFormatting sqref="H168:H171">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4095,7 +4826,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H130:H132">
+  <conditionalFormatting sqref="H176:H179">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Point release for 0.78
Fixed the following:
After Reorder - Order Summary Page showing original items and not new items after changes made to details

After Reorder - Details Tab will not edit and save

Order Summary Screen - Mouse Wheel not working to scroll summary screen

Correspondecnce page would not save

After Reorder - Reorder would not give the next Order Number

Reorder on a Order Type of 'Embroidery Reorder' reverts to 'Screenprinting Reorder'

Order Page / Customers Tab - Customer Details Screen - Customer name is displaying 'false' instead of customer name
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA6E3CC8-7B69-421B-BFF8-8020BFC0AFED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B73808E-C630-44A4-9D7C-C5549DCC1060}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{AFF0B8A1-9626-46B3-9A62-F42AFA134D79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{AFF0B8A1-9626-46B3-9A62-F42AFA134D79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$21</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="200">
   <si>
     <t>Test Case</t>
   </si>
@@ -514,13 +518,126 @@
   </si>
   <si>
     <t>Delete Order Line Item (Red Trashcan)</t>
+  </si>
+  <si>
+    <t>After Reorder - Details Tab will not edit and save</t>
+  </si>
+  <si>
+    <t>After Reorder - Order Summary Page showing original items and not new items after changes made to details</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Order Summary Screen - Mouse Wheel not working to scroll summary screen</t>
+  </si>
+  <si>
+    <t>Did not require any code update</t>
+  </si>
+  <si>
+    <t>Correspondecnce page would not save</t>
+  </si>
+  <si>
+    <t>Minor Code fix needed for Orders that don't have a Billing Address 1 for the order.</t>
+  </si>
+  <si>
+    <t>After Reorder - Reorder would not give the next Order Number</t>
+  </si>
+  <si>
+    <t>Reorder on a Order Type of 'Embroidery Reorder' reverts to 'Screenprinting Reorder'</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Could be Related to error where 'tax_rate' is null.</t>
+  </si>
+  <si>
+    <t>Updated logic to check for original (new) orders and set to Reorder version.  If it is not found, then the reorder will be the same order type as the original order.</t>
+  </si>
+  <si>
+    <t>New orders not showing up in list</t>
+  </si>
+  <si>
+    <t>Recreation</t>
+  </si>
+  <si>
+    <t>Need to recreate.  When I test, I see the orders in the list.</t>
+  </si>
+  <si>
+    <t>Garments Page - Order not showing up under the 'Today' Filter</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Orders only show up on Garment order Page's 'Today' filter if the garments for that order were ordered 'Today'</t>
+  </si>
+  <si>
+    <t>Order Page / Customers Tab - Customer Details Screen - Customer naem is displaying 'false' instead of customer name</t>
+  </si>
+  <si>
+    <t>Added to display on Order list tab</t>
+  </si>
+  <si>
+    <t>New Order - Order Number Generation - Order number is not Generated until the order is saved.</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>If we need to generate the order number before the order is saved, then there will be a good amount of coding required on both the front end and database end of the system.  The old system used HotJas to generate the number.</t>
+  </si>
+  <si>
+    <t>New Order - Order not saving on first try</t>
+  </si>
+  <si>
+    <t>Need to recreate.  When I test, I have no issue saving.  Need to see exactly what was entered so we can determine if a specific field in the order is causing the issue.</t>
+  </si>
+  <si>
+    <t>New Customer - Issue when Clicking on the '+' button while there is something in the search bar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation </t>
+  </si>
+  <si>
+    <t>New Customer - Can only setup new Customer under 'contacts' tab and not under 'customers' tab.</t>
+  </si>
+  <si>
+    <t>Order Details Tab - Detail Line Items order is inconsistent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When keying in the line items, things go in a weird order in sims 2.  In sims 1 when you copy a line, it copies and goes to the bottom of the page (which it should).
+In sims 2 when you copy a line, it deletes line 1 and shifts everything down a notch.  When I saved a correspondence, it scrambled up the line items and on the order summary it didn't save any edits.  In the new sims, the details page should always save the changes and carry over perfectly into the order summary page as well as the correspondence page.  This is highly important and really needs to be accurate
+</t>
+  </si>
+  <si>
+    <t>Enhancement</t>
+  </si>
+  <si>
+    <t>I'll see what I can do, it may require a lot more coding.</t>
+  </si>
+  <si>
+    <t>Search Parameters on grids don't persist on a page refresh.</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,8 +660,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,8 +706,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -708,11 +839,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -774,6 +950,34 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1443,7 +1647,7 @@
   </sheetPr>
   <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E181" sqref="E181"/>
     </sheetView>
   </sheetViews>
@@ -4837,4 +5041,279 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27DE111-B634-4CDA-84A0-4AC836C76705}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" style="37" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" style="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42">
+        <v>1</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39">
+        <v>2</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39">
+        <v>3</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="41"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39">
+        <v>4</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39">
+        <v>5</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="39">
+        <v>7</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="39">
+        <v>8</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39">
+        <v>9</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="39">
+        <v>10</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
+        <v>11</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="39">
+        <v>12</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="41"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="39">
+        <v>13</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A15" s="39">
+        <v>14</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="39">
+        <v>15</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D21" xr:uid="{34CCC53E-8684-4327-9173-EAF7B85C639F}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Discuss"/>
+        <filter val="Enhancement"/>
+        <filter val="In Progress"/>
+        <filter val="Recreation"/>
+        <filter val="Rejected"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ver 0.78 - Last Minute Fix
Componetized the Customer Popup Screen for consistancy.  Updated code to initialize new customer to make it the same when called from the Contact or Customer screen.
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B73808E-C630-44A4-9D7C-C5549DCC1060}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE2FD7D-1A55-4FFF-B502-BD91DE7D20C6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{AFF0B8A1-9626-46B3-9A62-F42AFA134D79}"/>
   </bookViews>
@@ -580,9 +580,6 @@
     <t>Orders only show up on Garment order Page's 'Today' filter if the garments for that order were ordered 'Today'</t>
   </si>
   <si>
-    <t>Order Page / Customers Tab - Customer Details Screen - Customer naem is displaying 'false' instead of customer name</t>
-  </si>
-  <si>
     <t>Added to display on Order list tab</t>
   </si>
   <si>
@@ -631,6 +628,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Order Page / Customers Tab - Customer Details Screen - Customer name is displaying 'false' instead of customer name</t>
   </si>
 </sst>
 </file>
@@ -5045,11 +5045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27DE111-B634-4CDA-84A0-4AC836C76705}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5062,10 +5061,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>198</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>199</v>
       </c>
       <c r="C1" s="47" t="s">
         <v>165</v>
@@ -5074,7 +5073,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="42">
         <v>1</v>
       </c>
@@ -5086,7 +5085,7 @@
       </c>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>2</v>
       </c>
@@ -5100,7 +5099,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -5112,7 +5111,7 @@
       </c>
       <c r="D4" s="41"/>
     </row>
-    <row r="5" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>4</v>
       </c>
@@ -5126,7 +5125,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -5140,7 +5139,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="39">
         <v>6</v>
       </c>
@@ -5182,18 +5181,18 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <v>9</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>167</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -5201,13 +5200,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="D11" s="41" t="s">
         <v>186</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -5215,13 +5214,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>178</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5229,10 +5228,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" s="39" t="s">
         <v>190</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>191</v>
       </c>
       <c r="D13" s="41"/>
     </row>
@@ -5241,7 +5240,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C14" s="39" t="s">
         <v>174</v>
@@ -5253,13 +5252,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="39" t="s">
         <v>174</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5267,52 +5266,42 @@
         <v>15</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C16" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="D16" s="41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D21" xr:uid="{34CCC53E-8684-4327-9173-EAF7B85C639F}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Discuss"/>
-        <filter val="Enhancement"/>
-        <filter val="In Progress"/>
-        <filter val="Recreation"/>
-        <filter val="Rejected"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D21" xr:uid="{34CCC53E-8684-4327-9173-EAF7B85C639F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes for issues found during general testing.
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\SouthPaw\SIMSRewrite\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFAAADB-8607-4BA3-BE76-14BC32A8280A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$21</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="200">
   <si>
     <t>Test Case</t>
   </si>
@@ -550,9 +551,6 @@
   </si>
   <si>
     <t>Reorder on a Order Type of 'Embroidery Reorder' reverts to 'Screenprinting Reorder'</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Could be Related to error where 'tax_rate' is null.</t>
@@ -629,12 +627,15 @@
   <si>
     <t>For Line Items, Add to Top of list and keep (copy) Item Desc, Color, Vendor, Manfuacturer, Style #, Price.
 For Art Placement, Add to end of list.</t>
+  </si>
+  <si>
+    <t>Version Fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,7 +712,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -882,11 +883,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -978,6 +992,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,7 +1342,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="33"/>
       <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
@@ -1639,7 +1654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5042,36 +5057,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="56.85546875" style="37" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" style="38" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>193</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>194</v>
       </c>
       <c r="C1" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="48" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="42">
         <v>1</v>
       </c>
@@ -5081,9 +5099,12 @@
       <c r="C2" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="44"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="42">
+        <v>0.78</v>
+      </c>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>2</v>
       </c>
@@ -5093,11 +5114,14 @@
       <c r="C3" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42">
+        <v>0.78</v>
+      </c>
+      <c r="E3" s="41" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -5107,9 +5131,12 @@
       <c r="C4" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="41"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="42">
+        <v>0.78</v>
+      </c>
+      <c r="E4" s="41"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>4</v>
       </c>
@@ -5119,11 +5146,14 @@
       <c r="C5" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="42">
+        <v>0.78</v>
+      </c>
+      <c r="E5" s="41" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -5133,11 +5163,14 @@
       <c r="C6" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D6" s="42">
+        <v>0.78</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="39">
         <v>6</v>
       </c>
@@ -5147,132 +5180,154 @@
       <c r="C7" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="41" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="42">
+        <v>0.78</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>7</v>
       </c>
       <c r="B8" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="D8" s="39"/>
+      <c r="E8" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="D8" s="41" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>8</v>
       </c>
       <c r="B9" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="D9" s="39"/>
+      <c r="E9" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="D9" s="41" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <v>9</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="D10" s="39">
+        <v>0.78</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>10</v>
       </c>
       <c r="B11" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>196</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>11</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D12" s="41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" s="39">
+        <v>0.78</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
         <v>12</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D13" s="41"/>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="39">
+        <v>0.78</v>
+      </c>
+      <c r="E13" s="41"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
         <v>13</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C14" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D14" s="41" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D14" s="39">
+        <v>0.78</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
         <v>14</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="D15" s="39">
+        <v>0.79</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
         <v>15</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="41" t="s">
         <v>190</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -5301,7 +5356,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D21"/>
+  <autoFilter ref="A1:E21" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update from Client Visit. Ver 0.79
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\SouthPaw\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BD7FD8-99E7-4CBB-87CF-10E60104480A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$22</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="218">
   <si>
     <t>Test Case</t>
   </si>
@@ -560,9 +559,6 @@
   </si>
   <si>
     <t>New orders not showing up in list</t>
-  </si>
-  <si>
-    <t>Recreation</t>
   </si>
   <si>
     <t>Need to recreate.  When I test, I see the orders in the list.</t>
@@ -665,16 +661,34 @@
     <t>New Order - Order Invoice does not display</t>
   </si>
   <si>
-    <t>Need recreation steps.  When I generate one, even with no details, the invoice displays.</t>
-  </si>
-  <si>
     <t>ReOrder - Order Details Tab - Detail items not being duplicated on Save</t>
+  </si>
+  <si>
+    <t>Order Summary Screen - Mouse Wheel not working to scroll summary screen when brought up by Order Page</t>
+  </si>
+  <si>
+    <t>Order Summary Screen - Remove Duplicate headers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Art Placement and Quantity Header is showing up per line item </t>
+  </si>
+  <si>
+    <t>Order Page - Reorder Function - After editing details with multiple line items, on Save, Order of Detailed line items switches</t>
+  </si>
+  <si>
+    <t>Change one Line Item in multi line item order and save.  Order will not be consistent.  Need to provide order by function in pull.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order Summary Screen - Item Type is not displaying </t>
+  </si>
+  <si>
+    <t>Issue was with details array.  Should be fixed now.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -708,7 +722,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -976,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1046,13 +1060,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1062,19 +1069,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1096,6 +1095,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1454,7 +1460,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="33"/>
       <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
@@ -1766,7 +1772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5169,11 +5175,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="B24" sqref="B23:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5185,363 +5191,429 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="C1" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="56">
+        <v>1</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="56">
+        <v>0.78</v>
+      </c>
+      <c r="E2" s="58"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>2</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="56">
+        <v>0.78</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="44">
+        <v>3</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="56">
+        <v>0.78</v>
+      </c>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>4</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="56">
+        <v>0.78</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
+        <v>5</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="56">
+        <v>0.78</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="44">
+        <v>6</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="56">
+        <v>0.78</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="44">
+        <v>7</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="59">
+        <v>8</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="E9" s="61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="44">
+        <v>9</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" s="46" t="s">
+      <c r="C10" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
+        <v>10</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="E11" s="46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="44">
+        <v>11</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="44">
+        <v>12</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="E13" s="46"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="44">
+        <v>13</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="47">
+        <v>14</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="47">
+        <v>0.79</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="50">
+        <v>15</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="52" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="53">
+        <v>16</v>
+      </c>
+      <c r="B17" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="45" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="51">
-        <v>1</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="E2" s="53"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="54">
-        <v>2</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="E3" s="56" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="54">
-        <v>3</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="E4" s="56"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="54">
-        <v>4</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="E5" s="56" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="54">
-        <v>5</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D6" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="54">
-        <v>6</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="48">
-        <v>7</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" s="48">
-        <v>0.78</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="63">
-        <v>8</v>
-      </c>
-      <c r="B9" s="64" t="s">
+      <c r="C17" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="E17" s="55" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="44">
+        <v>17</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="44"/>
+      <c r="E18" s="46" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="53">
+        <v>18</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="53">
+        <v>0.8</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="44">
+        <v>19</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="44">
+        <v>0.79</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="59">
+        <v>20</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" s="59" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="63" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="65" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="54">
-        <v>9</v>
-      </c>
-      <c r="B10" s="55" t="s">
+      <c r="D21" s="59">
+        <v>0.79</v>
+      </c>
+      <c r="E21" s="61" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="44">
+        <v>21</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="54">
-        <v>0.78</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="48">
-        <v>10</v>
-      </c>
-      <c r="B11" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="50" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="54">
-        <v>11</v>
-      </c>
-      <c r="B12" s="55" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" s="54">
-        <v>0.78</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="54">
-        <v>12</v>
-      </c>
-      <c r="B13" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" s="54">
-        <v>0.78</v>
-      </c>
-      <c r="E13" s="56"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="54">
-        <v>13</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>187</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="54">
-        <v>0.78</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="54">
-        <v>14</v>
-      </c>
-      <c r="B15" s="55" t="s">
-        <v>188</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D15" s="54">
+      <c r="D22" s="44">
         <v>0.79</v>
       </c>
-      <c r="E15" s="56" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="57">
-        <v>15</v>
-      </c>
-      <c r="B16" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="C16" s="57" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" s="57"/>
-      <c r="E16" s="59" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="60">
-        <v>16</v>
-      </c>
-      <c r="B17" s="61" t="s">
+      <c r="E22" s="46" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="44">
+        <v>22</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="44">
+        <v>0.79</v>
+      </c>
+      <c r="E23" s="46"/>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="53">
+        <v>23</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="62" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
-        <v>17</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>212</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="41" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="54">
-        <v>18</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>204</v>
-      </c>
-      <c r="C19" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D19" s="54">
-        <v>0.79</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="54">
-        <v>19</v>
-      </c>
-      <c r="B20" s="55" t="s">
-        <v>206</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="54">
-        <v>0.79</v>
-      </c>
-      <c r="E20" s="56" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="63">
-        <v>20</v>
-      </c>
-      <c r="B21" s="64" t="s">
-        <v>208</v>
-      </c>
-      <c r="C21" s="63" t="s">
-        <v>180</v>
-      </c>
-      <c r="D21" s="63">
-        <v>0.79</v>
-      </c>
-      <c r="E21" s="65" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="47">
-        <v>21</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>210</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="41" t="s">
-        <v>211</v>
-      </c>
+      <c r="D24" s="53">
+        <v>0.8</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="53">
+        <v>24</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" s="53">
+        <v>0.8</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="53">
+        <v>25</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" s="53">
+        <v>0.8</v>
+      </c>
+      <c r="E26" s="55"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E22" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:E22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 0.8 start fixes
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\SouthPaw\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D06DFF-E111-4CC7-B7C5-503950F63598}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="223">
   <si>
     <t>Test Case</t>
   </si>
@@ -682,12 +681,30 @@
   <si>
     <t>Change one Line Item in multi line item order and save.  Order will not be consistent.  Need to provide order by function in pull.  
 RWF - Added sort of item.  When adding item, new one shows on top and then on save it moves to the end of the list.  Need to know if this acceptable functionality.</t>
+  </si>
+  <si>
+    <t>Garments Page - Default Filter Performance</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Default Filter is timing out on return of Garment Data</t>
+  </si>
+  <si>
+    <t>Order Invoice - Order Date, Due Date, PO#, and Sale Rep Values are shifted down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Invoice for details.  </t>
+  </si>
+  <si>
+    <t>Order Invoice - Add Periods to end of footer text.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -778,12 +795,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -791,6 +802,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1076,13 +1093,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1090,11 +1100,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1446,7 +1463,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="33"/>
       <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
@@ -1758,7 +1775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5161,11 +5178,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5194,19 +5211,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="53">
+      <c r="A2" s="50">
         <v>1</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="50">
         <v>0.78</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="44">
@@ -5218,7 +5235,7 @@
       <c r="C3" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="50">
         <v>0.78</v>
       </c>
       <c r="E3" s="46" t="s">
@@ -5235,7 +5252,7 @@
       <c r="C4" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="50">
         <v>0.78</v>
       </c>
       <c r="E4" s="46"/>
@@ -5250,7 +5267,7 @@
       <c r="C5" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="50">
         <v>0.78</v>
       </c>
       <c r="E5" s="46" t="s">
@@ -5267,7 +5284,7 @@
       <c r="C6" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="50">
         <v>0.78</v>
       </c>
       <c r="E6" s="46" t="s">
@@ -5284,7 +5301,7 @@
       <c r="C7" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="50">
         <v>0.78</v>
       </c>
       <c r="E7" s="46" t="s">
@@ -5309,17 +5326,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
+      <c r="A9" s="53">
         <v>8</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="58" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="55" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5363,7 +5380,7 @@
         <v>184</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="D12" s="44">
         <v>0.78</v>
@@ -5380,7 +5397,7 @@
         <v>185</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="D13" s="44">
         <v>0.78</v>
@@ -5395,7 +5412,7 @@
         <v>186</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="D14" s="44">
         <v>0.78</v>
@@ -5405,49 +5422,51 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+      <c r="A15" s="44">
         <v>14</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="C15" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D15" s="47">
+      <c r="C15" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="44">
         <v>0.79</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="46" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="50">
+      <c r="A16" s="47">
         <v>15</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="52" t="s">
+      <c r="D16" s="47"/>
+      <c r="E16" s="49" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="47">
+      <c r="A17" s="44">
         <v>16</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="49" t="s">
+      <c r="C17" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="E17" s="46" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5461,25 +5480,27 @@
       <c r="C18" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="D18" s="44"/>
+      <c r="D18" s="44">
+        <v>0.8</v>
+      </c>
       <c r="E18" s="46" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
+      <c r="A19" s="44">
         <v>18</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="C19" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D19" s="47">
+      <c r="C19" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="44">
         <v>0.8</v>
       </c>
-      <c r="E19" s="49" t="s">
+      <c r="E19" s="46" t="s">
         <v>203</v>
       </c>
     </row>
@@ -5501,19 +5522,19 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="56">
+      <c r="A21" s="53">
         <v>20</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="D21" s="56">
+      <c r="D21" s="53">
         <v>0.79</v>
       </c>
-      <c r="E21" s="58" t="s">
+      <c r="E21" s="55" t="s">
         <v>207</v>
       </c>
     </row>
@@ -5550,56 +5571,101 @@
       <c r="E23" s="46"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="47">
+      <c r="A24" s="44">
         <v>23</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="C24" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D24" s="47">
+      <c r="C24" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="44">
         <v>0.8</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="46" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="47">
+      <c r="A25" s="44">
         <v>24</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="C25" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D25" s="47">
+      <c r="C25" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D25" s="44">
         <v>0.8</v>
       </c>
-      <c r="E25" s="49" t="s">
+      <c r="E25" s="46" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="47">
+      <c r="A26" s="44">
         <v>25</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="C26" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D26" s="47">
+      <c r="C26" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="44">
         <v>0.8</v>
       </c>
-      <c r="E26" s="49"/>
+      <c r="E26" s="46"/>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="56">
+        <v>26</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" s="56"/>
+      <c r="E27" s="58" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="56">
+        <v>27</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" s="56"/>
+      <c r="E28" s="58" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="56">
+        <v>28</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D29" s="56"/>
+      <c r="E29" s="58" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E22" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:E22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 0.80 Sync After
Sync After all day session with Client
</commit_message>
<xml_diff>
--- a/docs/Test Scripts.xlsx
+++ b/docs/Test Scripts.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\South Paw\SIMSRewrite\SIMSRewrite\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\SouthPaw\SIMSRewrite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F75FDA1-0948-426E-B7DD-DAEA44373951}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$22</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="252">
   <si>
     <t>Test Case</t>
   </si>
@@ -702,16 +702,97 @@
     <t>Order Invoice - Add Periods to end of footer text.</t>
   </si>
   <si>
-    <t>Order Details Tab - ReOrder - Detail Lines not saving after editing data.</t>
-  </si>
-  <si>
-    <t>I used CAH Children's Attention Home embroidery reorder #0720201611 in sims 1.  I made edits to the details and it would not save.  After keying it in, I hit save and it defaulted back to the original line items on correspondence and order summary.  The order #121120181 was correct.  Task list was correct.  Basically, everything did right except for line items under details.  The art file was saved, the history/comments saved, I added a note and it showed up on the order summary, so that's good.  Then, I went back to the details to try to edit it again.  I deleted all of the line items except for the top line.  I then edited that top line item and saved.  When I did that, it defaulted back to the original top line.  However, it did save my deleted line changes, so that part worked.  It also saved 2 more edits...1. thread color that changed, and 2. the special charge I added for $5 under setup charges.  The correspondence and order summary showed the same things.....wrong item, but correct thread color and special $5 charge. In this scenario it appears that the details page is the only bug spot under line items.</t>
+    <t>Detail Task</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Customers - Customers</t>
+  </si>
+  <si>
+    <t>Functional Area (Page - Tab)</t>
+  </si>
+  <si>
+    <t>Customer Listing</t>
+  </si>
+  <si>
+    <t>Customer Search</t>
+  </si>
+  <si>
+    <t>Customer Creation</t>
+  </si>
+  <si>
+    <t>Customer Edit</t>
+  </si>
+  <si>
+    <t>Customers - Contacts</t>
+  </si>
+  <si>
+    <t>Sort order of Customer - Customer Page not sorting by Customer Name Ascending</t>
+  </si>
+  <si>
+    <t>Sort order of Customer - Contact Page not sorting by Customer Name Ascending</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Customer Page - Contact and Address Listing not consistent between deletes and saves</t>
+  </si>
+  <si>
+    <t>Customer - Customer - Orders</t>
+  </si>
+  <si>
+    <t>Order Listing</t>
+  </si>
+  <si>
+    <t>Order Search</t>
+  </si>
+  <si>
+    <t>Order Creation - Info</t>
+  </si>
+  <si>
+    <t>Order Creation - Tasks</t>
+  </si>
+  <si>
+    <t>Order Creation - Details</t>
+  </si>
+  <si>
+    <t>Order Creation - Art</t>
+  </si>
+  <si>
+    <t>Order Creation - History/Comments</t>
+  </si>
+  <si>
+    <t>Order Creation - Correspondence</t>
+  </si>
+  <si>
+    <t>Order Summary</t>
+  </si>
+  <si>
+    <t>Order Creation - Details - Payments</t>
+  </si>
+  <si>
+    <t>Order Creation  - Details - Line Item Order</t>
+  </si>
+  <si>
+    <t>Order Creation - Details - Art Placement Item order</t>
+  </si>
+  <si>
+    <t>Order Creation - Sales Tax</t>
+  </si>
+  <si>
+    <t>Customer - Contacts - Orders</t>
+  </si>
+  <si>
+    <t>Order Creation - Details - Line Copy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1013,7 +1094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1134,7 +1215,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1490,7 +1573,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="33"/>
       <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
@@ -1802,13 +1885,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E181" sqref="E181"/>
     </sheetView>
   </sheetViews>
@@ -5205,11 +5288,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:E30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5217,7 +5300,7 @@
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="56.85546875" style="37" customWidth="1"/>
     <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="75.140625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5656,111 +5739,569 @@
       <c r="C27" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="D27" s="56"/>
+      <c r="D27" s="56">
+        <v>0.81</v>
+      </c>
       <c r="E27" s="58" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="44">
+      <c r="A28" s="59">
         <v>27</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="60" t="s">
         <v>220</v>
       </c>
-      <c r="C28" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="46" t="s">
+      <c r="C28" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="59">
+        <v>0.81</v>
+      </c>
+      <c r="E28" s="61" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="44">
+      <c r="A29" s="59">
         <v>28</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="60" t="s">
         <v>222</v>
       </c>
-      <c r="C29" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="D29" s="44"/>
-      <c r="E29" s="46" t="s">
+      <c r="C29" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" s="59">
+        <v>0.81</v>
+      </c>
+      <c r="E29" s="61" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A30" s="59">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="64">
         <v>29</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="63">
+        <v>0.81</v>
+      </c>
+      <c r="E30" s="66"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="64">
+        <v>30</v>
+      </c>
+      <c r="B31" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="63">
+        <v>0.81</v>
+      </c>
+      <c r="E31" s="66"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="64">
+        <v>31</v>
+      </c>
+      <c r="B32" s="65" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="63">
+        <v>0.81</v>
+      </c>
+      <c r="E32" s="66"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="64">
+        <v>32</v>
+      </c>
+      <c r="B33" s="65"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="66"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="64">
+        <v>33</v>
+      </c>
+      <c r="B34" s="65"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="66"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="64">
+        <v>34</v>
+      </c>
+      <c r="B35" s="65"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="66"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E22"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="62" t="s">
         <v>223</v>
       </c>
-      <c r="C30" s="59" t="s">
-        <v>218</v>
-      </c>
-      <c r="D30" s="59">
-        <v>0.81</v>
-      </c>
-      <c r="E30" s="61" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="62">
+      <c r="D1" s="62" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="63">
+        <v>1</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="63">
+        <v>2</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="63">
+        <v>3</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="63">
+        <v>4</v>
+      </c>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="63">
+        <v>5</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="63">
+        <v>6</v>
+      </c>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="63">
+        <v>7</v>
+      </c>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="63">
+        <v>8</v>
+      </c>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="63">
+        <v>9</v>
+      </c>
+      <c r="B10" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>237</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="63">
+        <v>10</v>
+      </c>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="63">
+        <v>11</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="63">
+        <v>12</v>
+      </c>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="63">
+        <v>13</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="63">
+        <v>14</v>
+      </c>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="63">
+        <v>15</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="63">
+        <v>16</v>
+      </c>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="63">
+        <v>17</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="63">
+        <v>18</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="63">
+        <v>19</v>
+      </c>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="63">
+        <v>20</v>
+      </c>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="63">
+        <v>21</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="63">
+        <v>22</v>
+      </c>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63" t="s">
+        <v>251</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="63">
+        <v>23</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" s="63"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="63">
+        <v>24</v>
+      </c>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" s="63"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="63">
+        <v>25</v>
+      </c>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="63"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="63">
+        <v>26</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="D27" s="63"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="63">
+        <v>27</v>
+      </c>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63" t="s">
+        <v>241</v>
+      </c>
+      <c r="D28" s="63"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="63">
+        <v>28</v>
+      </c>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63" t="s">
+        <v>242</v>
+      </c>
+      <c r="D29" s="63"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="63">
+        <v>29</v>
+      </c>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63" t="s">
+        <v>243</v>
+      </c>
+      <c r="D30" s="63"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="63">
         <v>30</v>
       </c>
       <c r="B31" s="63"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="64"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
+      <c r="C31" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="D31" s="63"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="63">
+        <v>31</v>
+      </c>
       <c r="B32" s="63"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="64"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
+      <c r="C32" s="63" t="s">
+        <v>245</v>
+      </c>
+      <c r="D32" s="63"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="63">
+        <v>32</v>
+      </c>
       <c r="B33" s="63"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="64"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
+      <c r="C33" s="63" t="s">
+        <v>246</v>
+      </c>
+      <c r="D33" s="63"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="63">
+        <v>33</v>
+      </c>
       <c r="B34" s="63"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="64"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
+      <c r="C34" s="63" t="s">
+        <v>247</v>
+      </c>
+      <c r="D34" s="63"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="63">
+        <v>34</v>
+      </c>
       <c r="B35" s="63"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="64"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
+      <c r="C35" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" s="63"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="63">
+        <v>35</v>
+      </c>
       <c r="B36" s="63"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="64"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
+      <c r="C36" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="D36" s="63"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="63">
+        <v>36</v>
+      </c>
       <c r="B37" s="63"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="64"/>
+      <c r="C37" s="63" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="63"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E22" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>